<commit_message>
Ajuste no nome das sheet_name
</commit_message>
<xml_diff>
--- a/Automação/Comercial/Cadastro/BOT Cadastro/Cadastro JOANIN.xlsx
+++ b/Automação/Comercial/Cadastro/BOT Cadastro/Cadastro JOANIN.xlsx
@@ -6,9 +6,12 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="20370" yWindow="-2340" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="IQF AMORA CONGELADOS (1,200 KG)" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="POLPINHA DE ABACAXI (100G)" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="POLPINHA DE ACEROLA (100G)" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="9401" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="9398" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="9399" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="9626" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="9633" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="9634" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -1724,7 +1727,7 @@
       </c>
       <c r="C16" s="32" t="inlineStr">
         <is>
-          <t>IQF AMORA CONGELADOS (1,200 KG)</t>
+          <t>CONGELADO BROCOLIS DM (1,020KG)</t>
         </is>
       </c>
       <c r="D16" s="99" t="n"/>
@@ -1744,7 +1747,7 @@
       </c>
       <c r="C17" s="65" t="inlineStr">
         <is>
-          <t>7896519222483</t>
+          <t>7896519233106</t>
         </is>
       </c>
       <c r="D17" s="101" t="n"/>
@@ -1771,7 +1774,7 @@
       </c>
       <c r="C18" s="51" t="inlineStr">
         <is>
-          <t>1.2</t>
+          <t>1.02</t>
         </is>
       </c>
       <c r="D18" s="101" t="n"/>
@@ -1782,7 +1785,7 @@
       </c>
       <c r="F18" s="32" t="inlineStr">
         <is>
-          <t>1.2</t>
+          <t>1.026</t>
         </is>
       </c>
       <c r="G18" s="99" t="n"/>
@@ -1836,7 +1839,7 @@
       </c>
       <c r="C21" s="59" t="inlineStr">
         <is>
-          <t>0.315</t>
+          <t>0.35</t>
         </is>
       </c>
       <c r="D21" s="99" t="n"/>
@@ -1870,7 +1873,7 @@
       </c>
       <c r="C23" s="25" t="inlineStr">
         <is>
-          <t>34</t>
+          <t>9401</t>
         </is>
       </c>
       <c r="D23" s="106" t="n"/>
@@ -1928,7 +1931,7 @@
       </c>
       <c r="C27" s="34" t="inlineStr">
         <is>
-          <t>9.0</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="D27" s="99" t="n"/>
@@ -1947,7 +1950,7 @@
       </c>
       <c r="C28" s="63" t="inlineStr">
         <is>
-          <t>67896519222485</t>
+          <t>67896519233108</t>
         </is>
       </c>
       <c r="D28" s="99" t="n"/>
@@ -1966,7 +1969,7 @@
       </c>
       <c r="C29" s="34" t="inlineStr">
         <is>
-          <t>10.8</t>
+          <t>6.156</t>
         </is>
       </c>
       <c r="D29" s="99" t="n"/>
@@ -1985,7 +1988,7 @@
       </c>
       <c r="C30" s="32" t="inlineStr">
         <is>
-          <t>10.8</t>
+          <t>6.12</t>
         </is>
       </c>
       <c r="D30" s="99" t="n"/>
@@ -2004,7 +2007,7 @@
       </c>
       <c r="C31" s="34" t="inlineStr">
         <is>
-          <t>0.46</t>
+          <t>0.39</t>
         </is>
       </c>
       <c r="D31" s="99" t="n"/>
@@ -2023,7 +2026,7 @@
       </c>
       <c r="C32" s="32" t="inlineStr">
         <is>
-          <t>0.08</t>
+          <t>0.22</t>
         </is>
       </c>
       <c r="D32" s="99" t="n"/>
@@ -2042,7 +2045,7 @@
       </c>
       <c r="C33" s="25" t="inlineStr">
         <is>
-          <t>0.315</t>
+          <t>0.295</t>
         </is>
       </c>
       <c r="D33" s="106" t="n"/>
@@ -2222,7 +2225,7 @@
       </c>
       <c r="C47" s="32" t="inlineStr">
         <is>
-          <t>0811.20.00</t>
+          <t>0710.80.00</t>
         </is>
       </c>
       <c r="D47" s="99" t="n"/>
@@ -3055,7 +3058,7 @@
       </c>
       <c r="C16" s="32" t="inlineStr">
         <is>
-          <t>POLPINHA DE ABACAXI (100G)</t>
+          <t>CONGELADO JARDINEIRA S/ MILHO (1,020 KG)</t>
         </is>
       </c>
       <c r="D16" s="99" t="n"/>
@@ -3075,7 +3078,7 @@
       </c>
       <c r="C17" s="65" t="inlineStr">
         <is>
-          <t>7896519211036</t>
+          <t>7896519246182</t>
         </is>
       </c>
       <c r="D17" s="101" t="n"/>
@@ -3102,7 +3105,7 @@
       </c>
       <c r="C18" s="51" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1.02</t>
         </is>
       </c>
       <c r="D18" s="101" t="n"/>
@@ -3113,7 +3116,7 @@
       </c>
       <c r="F18" s="32" t="inlineStr">
         <is>
-          <t>1.05</t>
+          <t>1.026</t>
         </is>
       </c>
       <c r="G18" s="99" t="n"/>
@@ -3129,7 +3132,7 @@
       </c>
       <c r="C19" s="34" t="inlineStr">
         <is>
-          <t>0.24</t>
+          <t>0.46</t>
         </is>
       </c>
       <c r="D19" s="99" t="n"/>
@@ -3148,7 +3151,7 @@
       </c>
       <c r="C20" s="57" t="inlineStr">
         <is>
-          <t>0.19</t>
+          <t>0.08</t>
         </is>
       </c>
       <c r="D20" s="99" t="n"/>
@@ -3167,7 +3170,7 @@
       </c>
       <c r="C21" s="59" t="inlineStr">
         <is>
-          <t>0.21</t>
+          <t>0.35</t>
         </is>
       </c>
       <c r="D21" s="99" t="n"/>
@@ -3201,7 +3204,7 @@
       </c>
       <c r="C23" s="25" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>9398</t>
         </is>
       </c>
       <c r="D23" s="106" t="n"/>
@@ -3240,7 +3243,7 @@
       </c>
       <c r="C26" s="32" t="inlineStr">
         <is>
-          <t>KG</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="D26" s="99" t="n"/>
@@ -3259,7 +3262,7 @@
       </c>
       <c r="C27" s="34" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>12.0</t>
         </is>
       </c>
       <c r="D27" s="99" t="n"/>
@@ -3278,7 +3281,7 @@
       </c>
       <c r="C28" s="63" t="inlineStr">
         <is>
-          <t>67896519211038</t>
+          <t>67896519246184</t>
         </is>
       </c>
       <c r="D28" s="99" t="n"/>
@@ -3297,7 +3300,7 @@
       </c>
       <c r="C29" s="34" t="inlineStr">
         <is>
-          <t>6.3</t>
+          <t>12.312</t>
         </is>
       </c>
       <c r="D29" s="99" t="n"/>
@@ -3316,7 +3319,7 @@
       </c>
       <c r="C30" s="32" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>12.24</t>
         </is>
       </c>
       <c r="D30" s="99" t="n"/>
@@ -3335,7 +3338,7 @@
       </c>
       <c r="C31" s="34" t="inlineStr">
         <is>
-          <t>0.24</t>
+          <t>0.39</t>
         </is>
       </c>
       <c r="D31" s="99" t="n"/>
@@ -3354,7 +3357,7 @@
       </c>
       <c r="C32" s="32" t="inlineStr">
         <is>
-          <t>0.19</t>
+          <t>0.22</t>
         </is>
       </c>
       <c r="D32" s="99" t="n"/>
@@ -3373,7 +3376,7 @@
       </c>
       <c r="C33" s="25" t="inlineStr">
         <is>
-          <t>0.21</t>
+          <t>0.295</t>
         </is>
       </c>
       <c r="D33" s="106" t="n"/>
@@ -3553,7 +3556,7 @@
       </c>
       <c r="C47" s="32" t="inlineStr">
         <is>
-          <t>0811.90.00</t>
+          <t>0710.90.00</t>
         </is>
       </c>
       <c r="D47" s="99" t="n"/>
@@ -3572,7 +3575,7 @@
       </c>
       <c r="C48" s="34" t="inlineStr">
         <is>
-          <t>060</t>
+          <t>040</t>
         </is>
       </c>
       <c r="D48" s="99" t="n"/>
@@ -4386,7 +4389,7 @@
       </c>
       <c r="C16" s="32" t="inlineStr">
         <is>
-          <t>POLPINHA DE ACEROLA (100G)</t>
+          <t>CONGELADO LEGUMES PARA SALTEAR (1,020KG)</t>
         </is>
       </c>
       <c r="D16" s="99" t="n"/>
@@ -4406,7 +4409,7 @@
       </c>
       <c r="C17" s="65" t="inlineStr">
         <is>
-          <t>7896519210206</t>
+          <t>7896519246502</t>
         </is>
       </c>
       <c r="D17" s="101" t="n"/>
@@ -4433,7 +4436,7 @@
       </c>
       <c r="C18" s="51" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1.02</t>
         </is>
       </c>
       <c r="D18" s="101" t="n"/>
@@ -4444,7 +4447,7 @@
       </c>
       <c r="F18" s="32" t="inlineStr">
         <is>
-          <t>1.05</t>
+          <t>1.026</t>
         </is>
       </c>
       <c r="G18" s="99" t="n"/>
@@ -4460,7 +4463,7 @@
       </c>
       <c r="C19" s="34" t="inlineStr">
         <is>
-          <t>0.24</t>
+          <t>0.46</t>
         </is>
       </c>
       <c r="D19" s="99" t="n"/>
@@ -4479,7 +4482,7 @@
       </c>
       <c r="C20" s="57" t="inlineStr">
         <is>
-          <t>0.19</t>
+          <t>0.08</t>
         </is>
       </c>
       <c r="D20" s="99" t="n"/>
@@ -4498,7 +4501,7 @@
       </c>
       <c r="C21" s="59" t="inlineStr">
         <is>
-          <t>0.21</t>
+          <t>0.35</t>
         </is>
       </c>
       <c r="D21" s="99" t="n"/>
@@ -4532,7 +4535,7 @@
       </c>
       <c r="C23" s="25" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>9399</t>
         </is>
       </c>
       <c r="D23" s="106" t="n"/>
@@ -4571,7 +4574,7 @@
       </c>
       <c r="C26" s="32" t="inlineStr">
         <is>
-          <t>KG</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="D26" s="99" t="n"/>
@@ -4590,7 +4593,7 @@
       </c>
       <c r="C27" s="34" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="D27" s="99" t="n"/>
@@ -4609,7 +4612,7 @@
       </c>
       <c r="C28" s="63" t="inlineStr">
         <is>
-          <t>67896519210208</t>
+          <t>67896519246504</t>
         </is>
       </c>
       <c r="D28" s="99" t="n"/>
@@ -4628,7 +4631,7 @@
       </c>
       <c r="C29" s="34" t="inlineStr">
         <is>
-          <t>6.3</t>
+          <t>10.26</t>
         </is>
       </c>
       <c r="D29" s="99" t="n"/>
@@ -4647,7 +4650,7 @@
       </c>
       <c r="C30" s="32" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>10.2</t>
         </is>
       </c>
       <c r="D30" s="99" t="n"/>
@@ -4666,7 +4669,7 @@
       </c>
       <c r="C31" s="34" t="inlineStr">
         <is>
-          <t>0.24</t>
+          <t>0.39</t>
         </is>
       </c>
       <c r="D31" s="99" t="n"/>
@@ -4685,7 +4688,7 @@
       </c>
       <c r="C32" s="32" t="inlineStr">
         <is>
-          <t>0.19</t>
+          <t>0.22</t>
         </is>
       </c>
       <c r="D32" s="99" t="n"/>
@@ -4704,7 +4707,7 @@
       </c>
       <c r="C33" s="25" t="inlineStr">
         <is>
-          <t>0.21</t>
+          <t>0.295</t>
         </is>
       </c>
       <c r="D33" s="106" t="n"/>
@@ -4884,7 +4887,7 @@
       </c>
       <c r="C47" s="32" t="inlineStr">
         <is>
-          <t>0811.90.00</t>
+          <t>0710.90.00</t>
         </is>
       </c>
       <c r="D47" s="99" t="n"/>
@@ -4903,7 +4906,4000 @@
       </c>
       <c r="C48" s="34" t="inlineStr">
         <is>
-          <t>060</t>
+          <t>040</t>
+        </is>
+      </c>
+      <c r="D48" s="99" t="n"/>
+      <c r="E48" s="99" t="n"/>
+      <c r="F48" s="99" t="n"/>
+      <c r="G48" s="99" t="n"/>
+      <c r="H48" s="99" t="n"/>
+      <c r="I48" s="99" t="n"/>
+      <c r="J48" s="101" t="n"/>
+    </row>
+    <row r="49" ht="18" customHeight="1">
+      <c r="B49" s="3" t="inlineStr">
+        <is>
+          <t>IPI:</t>
+        </is>
+      </c>
+      <c r="C49" s="32" t="n"/>
+      <c r="D49" s="99" t="n"/>
+      <c r="E49" s="99" t="n"/>
+      <c r="F49" s="99" t="n"/>
+      <c r="G49" s="99" t="n"/>
+      <c r="H49" s="99" t="n"/>
+      <c r="I49" s="99" t="n"/>
+      <c r="J49" s="101" t="n"/>
+    </row>
+    <row r="50" ht="18" customHeight="1">
+      <c r="B50" s="5" t="inlineStr">
+        <is>
+          <t>ICMS ORIGEM:</t>
+        </is>
+      </c>
+      <c r="C50" s="44" t="n"/>
+      <c r="D50" s="99" t="n"/>
+      <c r="E50" s="99" t="n"/>
+      <c r="F50" s="99" t="n"/>
+      <c r="G50" s="99" t="n"/>
+      <c r="H50" s="99" t="n"/>
+      <c r="I50" s="99" t="n"/>
+      <c r="J50" s="101" t="n"/>
+    </row>
+    <row r="51" ht="18" customHeight="1">
+      <c r="B51" s="3" t="inlineStr">
+        <is>
+          <t>ICMS ENTRADA (SAIDA FORNEDOR):</t>
+        </is>
+      </c>
+      <c r="C51" s="46" t="n"/>
+      <c r="D51" s="101" t="n"/>
+      <c r="E51" s="4" t="inlineStr">
+        <is>
+          <t>CST ICMS</t>
+        </is>
+      </c>
+      <c r="F51" s="47" t="n"/>
+      <c r="G51" s="99" t="n"/>
+      <c r="H51" s="99" t="n"/>
+      <c r="I51" s="99" t="n"/>
+      <c r="J51" s="101" t="n"/>
+    </row>
+    <row r="52" ht="18" customHeight="1">
+      <c r="B52" s="5" t="inlineStr">
+        <is>
+          <t>REDUÇÃO DE ICMS:</t>
+        </is>
+      </c>
+      <c r="C52" s="49" t="n"/>
+      <c r="D52" s="99" t="n"/>
+      <c r="E52" s="99" t="n"/>
+      <c r="F52" s="99" t="n"/>
+      <c r="G52" s="99" t="n"/>
+      <c r="H52" s="99" t="n"/>
+      <c r="I52" s="99" t="n"/>
+      <c r="J52" s="101" t="n"/>
+    </row>
+    <row r="53" ht="18" customHeight="1">
+      <c r="B53" s="3" t="inlineStr">
+        <is>
+          <t>IVA%</t>
+        </is>
+      </c>
+      <c r="C53" s="32" t="n"/>
+      <c r="D53" s="99" t="n"/>
+      <c r="E53" s="99" t="n"/>
+      <c r="F53" s="99" t="n"/>
+      <c r="G53" s="99" t="n"/>
+      <c r="H53" s="99" t="n"/>
+      <c r="I53" s="99" t="n"/>
+      <c r="J53" s="101" t="n"/>
+    </row>
+    <row r="54" ht="18" customHeight="1">
+      <c r="B54" s="5" t="inlineStr">
+        <is>
+          <t>PAUTA%</t>
+        </is>
+      </c>
+      <c r="C54" s="34" t="n"/>
+      <c r="D54" s="99" t="n"/>
+      <c r="E54" s="99" t="n"/>
+      <c r="F54" s="99" t="n"/>
+      <c r="G54" s="99" t="n"/>
+      <c r="H54" s="99" t="n"/>
+      <c r="I54" s="99" t="n"/>
+      <c r="J54" s="101" t="n"/>
+    </row>
+    <row r="55" ht="18" customHeight="1">
+      <c r="B55" s="3" t="inlineStr">
+        <is>
+          <t>PIS%</t>
+        </is>
+      </c>
+      <c r="C55" s="42" t="n"/>
+      <c r="D55" s="101" t="n"/>
+      <c r="E55" s="4" t="inlineStr">
+        <is>
+          <t>CST PIS</t>
+        </is>
+      </c>
+      <c r="F55" s="42" t="n"/>
+      <c r="G55" s="99" t="n"/>
+      <c r="H55" s="99" t="n"/>
+      <c r="I55" s="99" t="n"/>
+      <c r="J55" s="101" t="n"/>
+    </row>
+    <row r="56" ht="18" customHeight="1" thickBot="1">
+      <c r="B56" s="7" t="inlineStr">
+        <is>
+          <t>COFINS%:</t>
+        </is>
+      </c>
+      <c r="C56" s="36" t="n"/>
+      <c r="D56" s="107" t="n"/>
+      <c r="E56" s="8" t="inlineStr">
+        <is>
+          <t>CST COFINS</t>
+        </is>
+      </c>
+      <c r="F56" s="36" t="n"/>
+      <c r="G56" s="106" t="n"/>
+      <c r="H56" s="106" t="n"/>
+      <c r="I56" s="106" t="n"/>
+      <c r="J56" s="107" t="n"/>
+    </row>
+    <row r="57" ht="18" customHeight="1" thickBot="1"/>
+    <row r="58" ht="18" customHeight="1">
+      <c r="B58" s="38" t="inlineStr">
+        <is>
+          <t>INFORMAÇÕES PREENCHIDAS PELA COMERCIAL OSWALDO CRUZ</t>
+        </is>
+      </c>
+      <c r="C58" s="93" t="n"/>
+      <c r="D58" s="93" t="n"/>
+      <c r="E58" s="93" t="n"/>
+      <c r="F58" s="93" t="n"/>
+      <c r="G58" s="93" t="n"/>
+      <c r="H58" s="93" t="n"/>
+      <c r="I58" s="93" t="n"/>
+      <c r="J58" s="94" t="n"/>
+    </row>
+    <row r="59" ht="18" customHeight="1">
+      <c r="B59" s="5" t="inlineStr">
+        <is>
+          <t>COMPRADOR:</t>
+        </is>
+      </c>
+      <c r="C59" s="34" t="n"/>
+      <c r="D59" s="99" t="n"/>
+      <c r="E59" s="99" t="n"/>
+      <c r="F59" s="99" t="n"/>
+      <c r="G59" s="99" t="n"/>
+      <c r="H59" s="99" t="n"/>
+      <c r="I59" s="99" t="n"/>
+      <c r="J59" s="101" t="n"/>
+    </row>
+    <row r="60" ht="18" customFormat="1" customHeight="1" s="9">
+      <c r="B60" s="3" t="inlineStr">
+        <is>
+          <t>MAPA:</t>
+        </is>
+      </c>
+      <c r="C60" s="41" t="inlineStr">
+        <is>
+          <t>A GRANDE (  )</t>
+        </is>
+      </c>
+      <c r="D60" s="115" t="n"/>
+      <c r="E60" s="41" t="inlineStr">
+        <is>
+          <t>A PEQUENO (  )</t>
+        </is>
+      </c>
+      <c r="F60" s="115" t="n"/>
+      <c r="G60" s="41" t="inlineStr">
+        <is>
+          <t>C GRANDE (  )</t>
+        </is>
+      </c>
+      <c r="H60" s="115" t="n"/>
+      <c r="I60" s="41" t="inlineStr">
+        <is>
+          <t>C PEQUENO (  )</t>
+        </is>
+      </c>
+      <c r="J60" s="14" t="n"/>
+    </row>
+    <row r="61" ht="18" customFormat="1" customHeight="1" s="9">
+      <c r="B61" s="5" t="inlineStr">
+        <is>
+          <t>ESTOQUES MÍNIMO E MÁXIMO:</t>
+        </is>
+      </c>
+      <c r="C61" s="6" t="inlineStr">
+        <is>
+          <t>MÍN:</t>
+        </is>
+      </c>
+      <c r="D61" s="6" t="inlineStr">
+        <is>
+          <t>MÁX:</t>
+        </is>
+      </c>
+      <c r="E61" s="6" t="inlineStr">
+        <is>
+          <t>MÍN:</t>
+        </is>
+      </c>
+      <c r="F61" s="6" t="inlineStr">
+        <is>
+          <t>MÁX:</t>
+        </is>
+      </c>
+      <c r="G61" s="6" t="inlineStr">
+        <is>
+          <t>MÍN:</t>
+        </is>
+      </c>
+      <c r="H61" s="6" t="inlineStr">
+        <is>
+          <t>MÁX:</t>
+        </is>
+      </c>
+      <c r="I61" s="6" t="inlineStr">
+        <is>
+          <t>MÍN:</t>
+        </is>
+      </c>
+      <c r="J61" s="15" t="inlineStr">
+        <is>
+          <t>MÁX:</t>
+        </is>
+      </c>
+    </row>
+    <row r="62" ht="18" customHeight="1">
+      <c r="B62" s="3" t="inlineStr">
+        <is>
+          <t>DISTRIBUIDO POR:</t>
+        </is>
+      </c>
+      <c r="C62" s="4" t="inlineStr">
+        <is>
+          <t>MATRIZ (  )</t>
+        </is>
+      </c>
+      <c r="D62" s="4" t="inlineStr">
+        <is>
+          <t>LOJA 05 (  )</t>
+        </is>
+      </c>
+      <c r="E62" s="4" t="inlineStr">
+        <is>
+          <t>LOJA 07 (  )</t>
+        </is>
+      </c>
+      <c r="F62" s="4" t="inlineStr">
+        <is>
+          <t>LOJA 20 (  )</t>
+        </is>
+      </c>
+      <c r="G62" s="4" t="inlineStr">
+        <is>
+          <t>LOJA 11(  )</t>
+        </is>
+      </c>
+      <c r="H62" s="4" t="n"/>
+      <c r="I62" s="4" t="n"/>
+      <c r="J62" s="14" t="n"/>
+    </row>
+    <row r="63" ht="18" customHeight="1">
+      <c r="B63" s="5" t="inlineStr">
+        <is>
+          <t>FORMA DE ABASTECIMENTO:</t>
+        </is>
+      </c>
+      <c r="C63" s="30" t="inlineStr">
+        <is>
+          <t>CENTRAL - CENTRAL (  )</t>
+        </is>
+      </c>
+      <c r="D63" s="115" t="n"/>
+      <c r="E63" s="30" t="inlineStr">
+        <is>
+          <t>CENTRAL - LOJA (  )</t>
+        </is>
+      </c>
+      <c r="F63" s="115" t="n"/>
+      <c r="G63" s="30" t="inlineStr">
+        <is>
+          <t>LOJA - LOJA (  )</t>
+        </is>
+      </c>
+      <c r="H63" s="115" t="n"/>
+      <c r="I63" s="30" t="inlineStr">
+        <is>
+          <t>CROSSDOCKING (  )</t>
+        </is>
+      </c>
+      <c r="J63" s="115" t="n"/>
+    </row>
+    <row r="64" ht="18" customHeight="1">
+      <c r="B64" s="3" t="inlineStr">
+        <is>
+          <t>JÁ EXISTE FAMÍLIA CADASTRADA?</t>
+        </is>
+      </c>
+      <c r="C64" s="32" t="n"/>
+      <c r="D64" s="99" t="n"/>
+      <c r="E64" s="99" t="n"/>
+      <c r="F64" s="99" t="n"/>
+      <c r="G64" s="99" t="n"/>
+      <c r="H64" s="99" t="n"/>
+      <c r="I64" s="99" t="n"/>
+      <c r="J64" s="101" t="n"/>
+    </row>
+    <row r="65" ht="18" customHeight="1">
+      <c r="B65" s="5" t="inlineStr">
+        <is>
+          <t>INFORME O CÓDIGO DA FAMÍLIA:</t>
+        </is>
+      </c>
+      <c r="C65" s="34" t="n"/>
+      <c r="D65" s="99" t="n"/>
+      <c r="E65" s="99" t="n"/>
+      <c r="F65" s="99" t="n"/>
+      <c r="G65" s="99" t="n"/>
+      <c r="H65" s="99" t="n"/>
+      <c r="I65" s="99" t="n"/>
+      <c r="J65" s="101" t="n"/>
+    </row>
+    <row r="66" ht="18" customHeight="1" thickBot="1">
+      <c r="B66" s="7" t="inlineStr">
+        <is>
+          <t>SEGMENTAÇÃO:</t>
+        </is>
+      </c>
+      <c r="C66" s="25" t="n"/>
+      <c r="D66" s="106" t="n"/>
+      <c r="E66" s="106" t="n"/>
+      <c r="F66" s="106" t="n"/>
+      <c r="G66" s="106" t="n"/>
+      <c r="H66" s="106" t="n"/>
+      <c r="I66" s="106" t="n"/>
+      <c r="J66" s="107" t="n"/>
+    </row>
+    <row r="67" ht="18" customHeight="1" thickBot="1">
+      <c r="B67" s="9" t="n"/>
+      <c r="E67" s="9" t="n"/>
+      <c r="F67" s="10" t="n"/>
+      <c r="G67" s="10" t="n"/>
+      <c r="H67" s="10" t="n"/>
+      <c r="I67" s="10" t="n"/>
+    </row>
+    <row r="68" ht="18" customHeight="1" thickBot="1">
+      <c r="B68" s="116" t="inlineStr">
+        <is>
+          <t>ATENÇÃO: TODO PRODUTO NOVO PRECISA DE UMA DIVISÃO INICIAL FEITA PELO COMPRADOR</t>
+        </is>
+      </c>
+      <c r="C68" s="117" t="n"/>
+      <c r="D68" s="117" t="n"/>
+      <c r="E68" s="117" t="n"/>
+      <c r="F68" s="117" t="n"/>
+      <c r="G68" s="117" t="n"/>
+      <c r="H68" s="117" t="n"/>
+      <c r="I68" s="117" t="n"/>
+      <c r="J68" s="118" t="n"/>
+    </row>
+    <row r="69" ht="18" customHeight="1"/>
+    <row r="70" ht="18" customHeight="1"/>
+    <row r="71" ht="18" customHeight="1">
+      <c r="B71" s="16" t="inlineStr">
+        <is>
+          <t>DATA</t>
+        </is>
+      </c>
+      <c r="C71" s="9" t="n"/>
+      <c r="D71" s="16" t="inlineStr">
+        <is>
+          <t>COMPRADOR</t>
+        </is>
+      </c>
+      <c r="E71" s="16" t="n"/>
+      <c r="F71" s="9" t="n"/>
+      <c r="G71" s="9" t="n"/>
+      <c r="H71" s="16" t="inlineStr">
+        <is>
+          <t>GERENTE COMPRAS</t>
+        </is>
+      </c>
+      <c r="I71" s="16" t="n"/>
+      <c r="J71" s="9" t="n"/>
+    </row>
+  </sheetData>
+  <mergeCells count="87">
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C33:J33"/>
+    <mergeCell ref="F10:J10"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="F6:J6"/>
+    <mergeCell ref="C20:J20"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="E63:F63"/>
+    <mergeCell ref="F18:J18"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="F8:J8"/>
+    <mergeCell ref="F17:J17"/>
+    <mergeCell ref="C59:J59"/>
+    <mergeCell ref="C52:J52"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F9:J9"/>
+    <mergeCell ref="B25:J25"/>
+    <mergeCell ref="C48:J48"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="C32:J32"/>
+    <mergeCell ref="F7:J7"/>
+    <mergeCell ref="C26:J26"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="F51:J51"/>
+    <mergeCell ref="C16:J16"/>
+    <mergeCell ref="C50:J50"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="B15:J15"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C28:J28"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="G60:H60"/>
+    <mergeCell ref="B58:J58"/>
+    <mergeCell ref="C30:J30"/>
+    <mergeCell ref="B42:J42"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="C64:J64"/>
+    <mergeCell ref="F55:J55"/>
+    <mergeCell ref="F12:J12"/>
+    <mergeCell ref="B35:J36"/>
+    <mergeCell ref="C54:J54"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C43:J43"/>
+    <mergeCell ref="F23:J23"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C27:J27"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="B46:J46"/>
+    <mergeCell ref="G63:H63"/>
+    <mergeCell ref="I63:J63"/>
+    <mergeCell ref="C66:J66"/>
+    <mergeCell ref="C19:J19"/>
+    <mergeCell ref="C53:J53"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C29:J29"/>
+    <mergeCell ref="C65:J65"/>
+    <mergeCell ref="C47:J47"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C44:J44"/>
+    <mergeCell ref="C22:J22"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="C31:J31"/>
+    <mergeCell ref="B68:J68"/>
+    <mergeCell ref="C21:J21"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="F13:J13"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="F56:J56"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="C49:J49"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
+  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B1:N71"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="1.5703125" customWidth="1" style="1" min="1" max="1"/>
+    <col width="33.28515625" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
+    <col width="15.7109375" customWidth="1" style="1" min="3" max="3"/>
+    <col width="14.7109375" customWidth="1" style="1" min="4" max="4"/>
+    <col width="23.7109375" customWidth="1" style="1" min="5" max="5"/>
+    <col width="14.7109375" customWidth="1" style="1" min="6" max="9"/>
+    <col width="11.5703125" customWidth="1" style="1" min="10" max="10"/>
+    <col width="9.140625" customWidth="1" style="1" min="11" max="16384"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="44.25" customHeight="1" thickBot="1">
+      <c r="B1" s="90" t="inlineStr">
+        <is>
+          <t>CADASTRO SUPERMERCADOS JOANIN LTDA</t>
+        </is>
+      </c>
+      <c r="C1" s="91" t="n"/>
+      <c r="D1" s="91" t="n"/>
+      <c r="E1" s="91" t="n"/>
+      <c r="F1" s="91" t="n"/>
+      <c r="G1" s="91" t="n"/>
+      <c r="H1" s="91" t="n"/>
+      <c r="I1" s="91" t="n"/>
+      <c r="J1" s="92" t="n"/>
+    </row>
+    <row r="2" ht="18" customHeight="1" thickBot="1"/>
+    <row r="3" ht="18" customHeight="1">
+      <c r="B3" s="38" t="inlineStr">
+        <is>
+          <t>INFORMAÇÕES FORNECEDOR</t>
+        </is>
+      </c>
+      <c r="C3" s="93" t="n"/>
+      <c r="D3" s="93" t="n"/>
+      <c r="E3" s="93" t="n"/>
+      <c r="F3" s="93" t="n"/>
+      <c r="G3" s="93" t="n"/>
+      <c r="H3" s="93" t="n"/>
+      <c r="I3" s="93" t="n"/>
+      <c r="J3" s="94" t="n"/>
+    </row>
+    <row r="4" ht="18" customHeight="1">
+      <c r="B4" s="95" t="inlineStr">
+        <is>
+          <t>É FORNECEDOR NOVO (    ) SIM     (   ) NÃO                           -                            FOI FEITO CONTRATO (   ) SIM      (    ) NÃO</t>
+        </is>
+      </c>
+      <c r="C4" s="96" t="n"/>
+      <c r="D4" s="96" t="n"/>
+      <c r="E4" s="96" t="n"/>
+      <c r="F4" s="96" t="n"/>
+      <c r="G4" s="96" t="n"/>
+      <c r="H4" s="96" t="n"/>
+      <c r="I4" s="96" t="n"/>
+      <c r="J4" s="97" t="n"/>
+    </row>
+    <row r="5" ht="18" customHeight="1">
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>RAZÃO SOCIAL:</t>
+        </is>
+      </c>
+      <c r="C5" s="98" t="inlineStr">
+        <is>
+          <t>NETFEIRA PONTOCOM LTDA</t>
+        </is>
+      </c>
+      <c r="D5" s="99" t="n"/>
+      <c r="E5" s="99" t="n"/>
+      <c r="F5" s="99" t="n"/>
+      <c r="G5" s="99" t="n"/>
+      <c r="H5" s="99" t="n"/>
+      <c r="I5" s="99" t="n"/>
+      <c r="J5" s="100" t="n"/>
+    </row>
+    <row r="6" ht="18" customHeight="1">
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+      <c r="C6" s="51" t="inlineStr">
+        <is>
+          <t>03.974.724/0001-24</t>
+        </is>
+      </c>
+      <c r="D6" s="101" t="n"/>
+      <c r="E6" s="4" t="inlineStr">
+        <is>
+          <t>INSC. ESTADUAL:</t>
+        </is>
+      </c>
+      <c r="F6" s="72" t="inlineStr">
+        <is>
+          <t>115.951.284-113</t>
+        </is>
+      </c>
+      <c r="G6" s="99" t="n"/>
+      <c r="H6" s="99" t="n"/>
+      <c r="I6" s="99" t="n"/>
+      <c r="J6" s="101" t="n"/>
+    </row>
+    <row r="7" ht="18" customHeight="1">
+      <c r="B7" s="5" t="inlineStr">
+        <is>
+          <t>ENDEREÇO:</t>
+        </is>
+      </c>
+      <c r="C7" s="71" t="inlineStr">
+        <is>
+          <t>AVENIDA DOUTOR GASTÃO VIDIGAL</t>
+        </is>
+      </c>
+      <c r="D7" s="101" t="n"/>
+      <c r="E7" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nº </t>
+        </is>
+      </c>
+      <c r="F7" s="72" t="inlineStr">
+        <is>
+          <t>1946</t>
+        </is>
+      </c>
+      <c r="G7" s="99" t="n"/>
+      <c r="H7" s="99" t="n"/>
+      <c r="I7" s="99" t="n"/>
+      <c r="J7" s="101" t="n"/>
+    </row>
+    <row r="8" ht="18" customHeight="1">
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BAIRRO: </t>
+        </is>
+      </c>
+      <c r="C8" s="51" t="inlineStr">
+        <is>
+          <t>VILA LEOPOLDINA</t>
+        </is>
+      </c>
+      <c r="D8" s="101" t="n"/>
+      <c r="E8" s="4" t="inlineStr">
+        <is>
+          <t>CEP:</t>
+        </is>
+      </c>
+      <c r="F8" s="72" t="inlineStr">
+        <is>
+          <t>5316900</t>
+        </is>
+      </c>
+      <c r="G8" s="99" t="n"/>
+      <c r="H8" s="99" t="n"/>
+      <c r="I8" s="99" t="n"/>
+      <c r="J8" s="101" t="n"/>
+    </row>
+    <row r="9" ht="18" customHeight="1">
+      <c r="B9" s="5" t="inlineStr">
+        <is>
+          <t>CIDADE:</t>
+        </is>
+      </c>
+      <c r="C9" s="34" t="inlineStr">
+        <is>
+          <t>SÃO PAULO</t>
+        </is>
+      </c>
+      <c r="D9" s="101" t="n"/>
+      <c r="E9" s="6" t="inlineStr">
+        <is>
+          <t>ESTADO:</t>
+        </is>
+      </c>
+      <c r="F9" s="71" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="G9" s="99" t="n"/>
+      <c r="H9" s="99" t="n"/>
+      <c r="I9" s="99" t="n"/>
+      <c r="J9" s="101" t="n"/>
+    </row>
+    <row r="10" ht="18" customHeight="1">
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>COMPLEMENTO:</t>
+        </is>
+      </c>
+      <c r="C10" s="51" t="inlineStr">
+        <is>
+          <t>P.AMA BOX 61/62,AMB BOX 3,4</t>
+        </is>
+      </c>
+      <c r="D10" s="101" t="n"/>
+      <c r="E10" s="19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PRAZO DE PGTO </t>
+        </is>
+      </c>
+      <c r="F10" s="102" t="n"/>
+      <c r="G10" s="99" t="n"/>
+      <c r="H10" s="99" t="n"/>
+      <c r="I10" s="99" t="n"/>
+      <c r="J10" s="100" t="n"/>
+    </row>
+    <row r="11" ht="18" customHeight="1">
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>CONTATO :</t>
+        </is>
+      </c>
+      <c r="C11" s="51" t="n"/>
+      <c r="D11" s="101" t="n"/>
+      <c r="E11" s="4" t="inlineStr">
+        <is>
+          <t>TELEFONE :</t>
+        </is>
+      </c>
+      <c r="F11" s="75" t="n"/>
+      <c r="G11" s="76" t="n"/>
+      <c r="H11" s="76" t="n"/>
+      <c r="I11" s="76" t="n"/>
+      <c r="J11" s="77" t="n"/>
+    </row>
+    <row r="12" ht="18" customHeight="1">
+      <c r="B12" s="23" t="inlineStr">
+        <is>
+          <t>E-MAIL PARA ENVIO XML</t>
+        </is>
+      </c>
+      <c r="C12" s="78" t="n"/>
+      <c r="D12" s="101" t="n"/>
+      <c r="E12" s="24" t="inlineStr">
+        <is>
+          <t>E-MAIL PARA FINANCEIRO</t>
+        </is>
+      </c>
+      <c r="F12" s="80" t="n"/>
+      <c r="G12" s="99" t="n"/>
+      <c r="H12" s="99" t="n"/>
+      <c r="I12" s="99" t="n"/>
+      <c r="J12" s="101" t="n"/>
+    </row>
+    <row r="13" ht="18" customHeight="1" thickBot="1">
+      <c r="B13" s="67" t="inlineStr">
+        <is>
+          <t>(    )COM INDENIZAÇÃO - FORNECEDOR ACEITA NOTA FISCAL DE DEVOLUÇÃO</t>
+        </is>
+      </c>
+      <c r="C13" s="103" t="n"/>
+      <c r="D13" s="103" t="n"/>
+      <c r="E13" s="103" t="n"/>
+      <c r="F13" s="70" t="inlineStr">
+        <is>
+          <t>(    ) SEM INDENIZAÇÃO  -  FORNECEDOR NÃO ACEITA NOTA FISCAL DEVOLUÇÃO</t>
+        </is>
+      </c>
+      <c r="G13" s="104" t="n"/>
+      <c r="H13" s="104" t="n"/>
+      <c r="I13" s="104" t="n"/>
+      <c r="J13" s="105" t="n"/>
+    </row>
+    <row r="14" ht="18" customHeight="1" thickBot="1">
+      <c r="B14" s="9" t="n"/>
+      <c r="E14" s="9" t="n"/>
+      <c r="F14" s="10" t="n"/>
+      <c r="G14" s="10" t="n"/>
+      <c r="H14" s="10" t="n"/>
+      <c r="I14" s="10" t="n"/>
+    </row>
+    <row r="15" ht="18" customHeight="1">
+      <c r="B15" s="38" t="inlineStr">
+        <is>
+          <t>DADOS DO PRODUTO - UNIDADE</t>
+        </is>
+      </c>
+      <c r="C15" s="93" t="n"/>
+      <c r="D15" s="93" t="n"/>
+      <c r="E15" s="93" t="n"/>
+      <c r="F15" s="93" t="n"/>
+      <c r="G15" s="93" t="n"/>
+      <c r="H15" s="93" t="n"/>
+      <c r="I15" s="93" t="n"/>
+      <c r="J15" s="94" t="n"/>
+    </row>
+    <row r="16" ht="18" customHeight="1">
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t>DESCRIÇÃO:</t>
+        </is>
+      </c>
+      <c r="C16" s="32" t="inlineStr">
+        <is>
+          <t>CONGELADO MIX DE LEGUMES (1,020KG )</t>
+        </is>
+      </c>
+      <c r="D16" s="99" t="n"/>
+      <c r="E16" s="99" t="n"/>
+      <c r="F16" s="99" t="n"/>
+      <c r="G16" s="99" t="n"/>
+      <c r="H16" s="99" t="n"/>
+      <c r="I16" s="99" t="n"/>
+      <c r="J16" s="101" t="n"/>
+      <c r="N16" s="11" t="n"/>
+    </row>
+    <row r="17" ht="18" customHeight="1">
+      <c r="B17" s="5" t="inlineStr">
+        <is>
+          <t>CÓD DE BARRAS:</t>
+        </is>
+      </c>
+      <c r="C17" s="65" t="inlineStr">
+        <is>
+          <t>7896519247042</t>
+        </is>
+      </c>
+      <c r="D17" s="101" t="n"/>
+      <c r="E17" s="12" t="inlineStr">
+        <is>
+          <t>MARCA:</t>
+        </is>
+      </c>
+      <c r="F17" s="65" t="inlineStr">
+        <is>
+          <t>DE MARCHI</t>
+        </is>
+      </c>
+      <c r="G17" s="99" t="n"/>
+      <c r="H17" s="99" t="n"/>
+      <c r="I17" s="99" t="n"/>
+      <c r="J17" s="101" t="n"/>
+    </row>
+    <row r="18" ht="18" customHeight="1">
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>PESO LIQUIDO KG:</t>
+        </is>
+      </c>
+      <c r="C18" s="51" t="inlineStr">
+        <is>
+          <t>1.02</t>
+        </is>
+      </c>
+      <c r="D18" s="101" t="n"/>
+      <c r="E18" s="4" t="inlineStr">
+        <is>
+          <t>PESO BRUTO KG:</t>
+        </is>
+      </c>
+      <c r="F18" s="32" t="inlineStr">
+        <is>
+          <t>1.07</t>
+        </is>
+      </c>
+      <c r="G18" s="99" t="n"/>
+      <c r="H18" s="99" t="n"/>
+      <c r="I18" s="99" t="n"/>
+      <c r="J18" s="101" t="n"/>
+    </row>
+    <row r="19" ht="18" customHeight="1">
+      <c r="B19" s="5" t="inlineStr">
+        <is>
+          <t>COMPRIMENTO EM CM:</t>
+        </is>
+      </c>
+      <c r="C19" s="34" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D19" s="99" t="n"/>
+      <c r="E19" s="99" t="n"/>
+      <c r="F19" s="99" t="n"/>
+      <c r="G19" s="99" t="n"/>
+      <c r="H19" s="99" t="n"/>
+      <c r="I19" s="99" t="n"/>
+      <c r="J19" s="101" t="n"/>
+    </row>
+    <row r="20" ht="18" customHeight="1">
+      <c r="B20" s="3" t="inlineStr">
+        <is>
+          <t>LARGURA EM CM:</t>
+        </is>
+      </c>
+      <c r="C20" s="57" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D20" s="99" t="n"/>
+      <c r="E20" s="99" t="n"/>
+      <c r="F20" s="99" t="n"/>
+      <c r="G20" s="99" t="n"/>
+      <c r="H20" s="99" t="n"/>
+      <c r="I20" s="99" t="n"/>
+      <c r="J20" s="101" t="n"/>
+    </row>
+    <row r="21" ht="18" customHeight="1">
+      <c r="B21" s="5" t="inlineStr">
+        <is>
+          <t>ALTURA EM CM:</t>
+        </is>
+      </c>
+      <c r="C21" s="59" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D21" s="99" t="n"/>
+      <c r="E21" s="99" t="n"/>
+      <c r="F21" s="99" t="n"/>
+      <c r="G21" s="99" t="n"/>
+      <c r="H21" s="99" t="n"/>
+      <c r="I21" s="99" t="n"/>
+      <c r="J21" s="101" t="n"/>
+    </row>
+    <row r="22" ht="18" customHeight="1">
+      <c r="B22" s="3" t="inlineStr">
+        <is>
+          <t>VALIDADE EM DIAS:</t>
+        </is>
+      </c>
+      <c r="C22" s="32" t="n"/>
+      <c r="D22" s="99" t="n"/>
+      <c r="E22" s="99" t="n"/>
+      <c r="F22" s="99" t="n"/>
+      <c r="G22" s="99" t="n"/>
+      <c r="H22" s="99" t="n"/>
+      <c r="I22" s="99" t="n"/>
+      <c r="J22" s="101" t="n"/>
+    </row>
+    <row r="23" ht="18" customHeight="1" thickBot="1">
+      <c r="B23" s="7" t="inlineStr">
+        <is>
+          <t>COD PRODUTO FORNECEDOR:</t>
+        </is>
+      </c>
+      <c r="C23" s="25" t="inlineStr">
+        <is>
+          <t>9626</t>
+        </is>
+      </c>
+      <c r="D23" s="106" t="n"/>
+      <c r="E23" s="107" t="n"/>
+      <c r="F23" s="61" t="inlineStr">
+        <is>
+          <t>(É OBRIGADOTÓRIO QUE O CÓDIGO DO FORNECEDOR SEJA O MESMO DO XML)</t>
+        </is>
+      </c>
+      <c r="G23" s="106" t="n"/>
+      <c r="H23" s="106" t="n"/>
+      <c r="I23" s="106" t="n"/>
+      <c r="J23" s="107" t="n"/>
+    </row>
+    <row r="24" ht="18" customHeight="1" thickBot="1"/>
+    <row r="25" ht="18" customHeight="1">
+      <c r="B25" s="38" t="inlineStr">
+        <is>
+          <t>DADOS DO PRODUTO - CAIXA</t>
+        </is>
+      </c>
+      <c r="C25" s="93" t="n"/>
+      <c r="D25" s="93" t="n"/>
+      <c r="E25" s="93" t="n"/>
+      <c r="F25" s="93" t="n"/>
+      <c r="G25" s="93" t="n"/>
+      <c r="H25" s="93" t="n"/>
+      <c r="I25" s="93" t="n"/>
+      <c r="J25" s="94" t="n"/>
+    </row>
+    <row r="26" ht="18" customHeight="1">
+      <c r="B26" s="3" t="inlineStr">
+        <is>
+          <t>TIPO DE EMBALAGEM:</t>
+        </is>
+      </c>
+      <c r="C26" s="32" t="inlineStr">
+        <is>
+          <t>UN</t>
+        </is>
+      </c>
+      <c r="D26" s="99" t="n"/>
+      <c r="E26" s="99" t="n"/>
+      <c r="F26" s="99" t="n"/>
+      <c r="G26" s="99" t="n"/>
+      <c r="H26" s="99" t="n"/>
+      <c r="I26" s="99" t="n"/>
+      <c r="J26" s="101" t="n"/>
+    </row>
+    <row r="27" ht="18" customHeight="1">
+      <c r="B27" s="5" t="inlineStr">
+        <is>
+          <t>QUANTIDADE NA CAIXA:</t>
+        </is>
+      </c>
+      <c r="C27" s="34" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="D27" s="99" t="n"/>
+      <c r="E27" s="99" t="n"/>
+      <c r="F27" s="99" t="n"/>
+      <c r="G27" s="99" t="n"/>
+      <c r="H27" s="99" t="n"/>
+      <c r="I27" s="99" t="n"/>
+      <c r="J27" s="101" t="n"/>
+    </row>
+    <row r="28" ht="18" customHeight="1">
+      <c r="B28" s="3" t="inlineStr">
+        <is>
+          <t>CÓD DUN:</t>
+        </is>
+      </c>
+      <c r="C28" s="63" t="inlineStr">
+        <is>
+          <t>67896519247044</t>
+        </is>
+      </c>
+      <c r="D28" s="99" t="n"/>
+      <c r="E28" s="99" t="n"/>
+      <c r="F28" s="99" t="n"/>
+      <c r="G28" s="99" t="n"/>
+      <c r="H28" s="99" t="n"/>
+      <c r="I28" s="99" t="n"/>
+      <c r="J28" s="101" t="n"/>
+    </row>
+    <row r="29" ht="18" customHeight="1">
+      <c r="B29" s="5" t="inlineStr">
+        <is>
+          <t>PESO BRUTO KG:</t>
+        </is>
+      </c>
+      <c r="C29" s="34" t="inlineStr">
+        <is>
+          <t>10.7</t>
+        </is>
+      </c>
+      <c r="D29" s="99" t="n"/>
+      <c r="E29" s="99" t="n"/>
+      <c r="F29" s="99" t="n"/>
+      <c r="G29" s="99" t="n"/>
+      <c r="H29" s="99" t="n"/>
+      <c r="I29" s="99" t="n"/>
+      <c r="J29" s="101" t="n"/>
+    </row>
+    <row r="30" ht="18" customHeight="1">
+      <c r="B30" s="3" t="inlineStr">
+        <is>
+          <t>PESO LIQUIDO KG:</t>
+        </is>
+      </c>
+      <c r="C30" s="32" t="inlineStr">
+        <is>
+          <t>10.2</t>
+        </is>
+      </c>
+      <c r="D30" s="99" t="n"/>
+      <c r="E30" s="99" t="n"/>
+      <c r="F30" s="99" t="n"/>
+      <c r="G30" s="99" t="n"/>
+      <c r="H30" s="99" t="n"/>
+      <c r="I30" s="99" t="n"/>
+      <c r="J30" s="101" t="n"/>
+    </row>
+    <row r="31" ht="18" customHeight="1">
+      <c r="B31" s="5" t="inlineStr">
+        <is>
+          <t>COMPRIMENTO EM CM:</t>
+        </is>
+      </c>
+      <c r="C31" s="34" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D31" s="99" t="n"/>
+      <c r="E31" s="99" t="n"/>
+      <c r="F31" s="99" t="n"/>
+      <c r="G31" s="99" t="n"/>
+      <c r="H31" s="99" t="n"/>
+      <c r="I31" s="99" t="n"/>
+      <c r="J31" s="101" t="n"/>
+    </row>
+    <row r="32" ht="18" customHeight="1">
+      <c r="B32" s="3" t="inlineStr">
+        <is>
+          <t>LARGURA EM CM:</t>
+        </is>
+      </c>
+      <c r="C32" s="32" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D32" s="99" t="n"/>
+      <c r="E32" s="99" t="n"/>
+      <c r="F32" s="99" t="n"/>
+      <c r="G32" s="99" t="n"/>
+      <c r="H32" s="99" t="n"/>
+      <c r="I32" s="99" t="n"/>
+      <c r="J32" s="101" t="n"/>
+    </row>
+    <row r="33" ht="18" customHeight="1" thickBot="1">
+      <c r="B33" s="7" t="inlineStr">
+        <is>
+          <t>ALTURA EM CM:</t>
+        </is>
+      </c>
+      <c r="C33" s="25" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D33" s="106" t="n"/>
+      <c r="E33" s="106" t="n"/>
+      <c r="F33" s="106" t="n"/>
+      <c r="G33" s="106" t="n"/>
+      <c r="H33" s="106" t="n"/>
+      <c r="I33" s="106" t="n"/>
+      <c r="J33" s="107" t="n"/>
+    </row>
+    <row r="34" ht="18" customHeight="1" thickBot="1"/>
+    <row r="35" ht="18" customHeight="1">
+      <c r="B35" s="38" t="inlineStr">
+        <is>
+          <t>CUSTO DO PRODUTO - UNITÁRIO</t>
+        </is>
+      </c>
+      <c r="C35" s="108" t="n"/>
+      <c r="D35" s="108" t="n"/>
+      <c r="E35" s="108" t="n"/>
+      <c r="F35" s="108" t="n"/>
+      <c r="G35" s="108" t="n"/>
+      <c r="H35" s="108" t="n"/>
+      <c r="I35" s="108" t="n"/>
+      <c r="J35" s="109" t="n"/>
+    </row>
+    <row r="36" ht="18" customHeight="1">
+      <c r="B36" s="110" t="n"/>
+      <c r="C36" s="111" t="n"/>
+      <c r="D36" s="111" t="n"/>
+      <c r="E36" s="111" t="n"/>
+      <c r="F36" s="111" t="n"/>
+      <c r="G36" s="111" t="n"/>
+      <c r="H36" s="111" t="n"/>
+      <c r="I36" s="111" t="n"/>
+      <c r="J36" s="112" t="n"/>
+    </row>
+    <row r="37" ht="18" customHeight="1">
+      <c r="B37" s="17" t="inlineStr">
+        <is>
+          <t>CUSTO SEM ST:</t>
+        </is>
+      </c>
+      <c r="C37" s="51" t="n"/>
+      <c r="D37" s="101" t="n"/>
+      <c r="E37" s="52" t="inlineStr">
+        <is>
+          <t>CUSTO COM ST:</t>
+        </is>
+      </c>
+      <c r="F37" s="113" t="n"/>
+      <c r="G37" s="51" t="n"/>
+      <c r="H37" s="101" t="n"/>
+      <c r="I37" s="52" t="n"/>
+      <c r="J37" s="113" t="n"/>
+    </row>
+    <row r="38" ht="18" customHeight="1">
+      <c r="B38" s="17" t="inlineStr">
+        <is>
+          <t>VALOR DA ST:</t>
+        </is>
+      </c>
+      <c r="C38" s="51" t="n"/>
+      <c r="D38" s="101" t="n"/>
+      <c r="E38" s="52" t="inlineStr">
+        <is>
+          <t>CUSTO UNITÁRIO FINAL:</t>
+        </is>
+      </c>
+      <c r="F38" s="113" t="n"/>
+      <c r="G38" s="51" t="n"/>
+      <c r="H38" s="101" t="n"/>
+      <c r="I38" s="52" t="n"/>
+      <c r="J38" s="113" t="n"/>
+    </row>
+    <row r="39" ht="18" customHeight="1">
+      <c r="B39" s="17" t="inlineStr">
+        <is>
+          <t>VERBA:</t>
+        </is>
+      </c>
+      <c r="C39" s="51" t="n"/>
+      <c r="D39" s="101" t="n"/>
+      <c r="E39" s="52" t="inlineStr">
+        <is>
+          <t>MARGEM:</t>
+        </is>
+      </c>
+      <c r="F39" s="113" t="n"/>
+      <c r="G39" s="51" t="n"/>
+      <c r="H39" s="101" t="n"/>
+      <c r="I39" s="52" t="n"/>
+      <c r="J39" s="113" t="n"/>
+    </row>
+    <row r="40" ht="18" customHeight="1" thickBot="1">
+      <c r="B40" s="18" t="n"/>
+      <c r="C40" s="53" t="n"/>
+      <c r="D40" s="107" t="n"/>
+      <c r="E40" s="54" t="inlineStr">
+        <is>
+          <t>VALOR DE VENDA:</t>
+        </is>
+      </c>
+      <c r="F40" s="114" t="n"/>
+      <c r="G40" s="53" t="n"/>
+      <c r="H40" s="107" t="n"/>
+      <c r="I40" s="54" t="n"/>
+      <c r="J40" s="114" t="n"/>
+    </row>
+    <row r="41" ht="18" customHeight="1" thickBot="1"/>
+    <row r="42" ht="18" customHeight="1">
+      <c r="B42" s="38" t="inlineStr">
+        <is>
+          <t>DADOS PALLETIZAÇÃO</t>
+        </is>
+      </c>
+      <c r="C42" s="93" t="n"/>
+      <c r="D42" s="93" t="n"/>
+      <c r="E42" s="93" t="n"/>
+      <c r="F42" s="93" t="n"/>
+      <c r="G42" s="93" t="n"/>
+      <c r="H42" s="93" t="n"/>
+      <c r="I42" s="93" t="n"/>
+      <c r="J42" s="94" t="n"/>
+    </row>
+    <row r="43" ht="18" customHeight="1">
+      <c r="B43" s="3" t="inlineStr">
+        <is>
+          <t>LASTRO/CAMADA:</t>
+        </is>
+      </c>
+      <c r="C43" s="32" t="n"/>
+      <c r="D43" s="99" t="n"/>
+      <c r="E43" s="99" t="n"/>
+      <c r="F43" s="99" t="n"/>
+      <c r="G43" s="99" t="n"/>
+      <c r="H43" s="99" t="n"/>
+      <c r="I43" s="99" t="n"/>
+      <c r="J43" s="101" t="n"/>
+    </row>
+    <row r="44" ht="18" customHeight="1" thickBot="1">
+      <c r="B44" s="7" t="inlineStr">
+        <is>
+          <t>ALTURA:</t>
+        </is>
+      </c>
+      <c r="C44" s="25" t="n"/>
+      <c r="D44" s="106" t="n"/>
+      <c r="E44" s="106" t="n"/>
+      <c r="F44" s="106" t="n"/>
+      <c r="G44" s="106" t="n"/>
+      <c r="H44" s="106" t="n"/>
+      <c r="I44" s="106" t="n"/>
+      <c r="J44" s="107" t="n"/>
+    </row>
+    <row r="45" ht="18" customHeight="1" thickBot="1"/>
+    <row r="46" ht="18" customHeight="1">
+      <c r="B46" s="38" t="inlineStr">
+        <is>
+          <t>INFORMAÇÕES FISCAIS</t>
+        </is>
+      </c>
+      <c r="C46" s="93" t="n"/>
+      <c r="D46" s="93" t="n"/>
+      <c r="E46" s="93" t="n"/>
+      <c r="F46" s="93" t="n"/>
+      <c r="G46" s="93" t="n"/>
+      <c r="H46" s="93" t="n"/>
+      <c r="I46" s="93" t="n"/>
+      <c r="J46" s="94" t="n"/>
+    </row>
+    <row r="47" ht="18" customHeight="1">
+      <c r="B47" s="3" t="inlineStr">
+        <is>
+          <t>NCM:</t>
+        </is>
+      </c>
+      <c r="C47" s="32" t="inlineStr">
+        <is>
+          <t>0710.90.00</t>
+        </is>
+      </c>
+      <c r="D47" s="99" t="n"/>
+      <c r="E47" s="99" t="n"/>
+      <c r="F47" s="99" t="n"/>
+      <c r="G47" s="99" t="n"/>
+      <c r="H47" s="99" t="n"/>
+      <c r="I47" s="99" t="n"/>
+      <c r="J47" s="101" t="n"/>
+    </row>
+    <row r="48" ht="18" customHeight="1">
+      <c r="B48" s="5" t="inlineStr">
+        <is>
+          <t>CEST:</t>
+        </is>
+      </c>
+      <c r="C48" s="34" t="inlineStr">
+        <is>
+          <t>040</t>
+        </is>
+      </c>
+      <c r="D48" s="99" t="n"/>
+      <c r="E48" s="99" t="n"/>
+      <c r="F48" s="99" t="n"/>
+      <c r="G48" s="99" t="n"/>
+      <c r="H48" s="99" t="n"/>
+      <c r="I48" s="99" t="n"/>
+      <c r="J48" s="101" t="n"/>
+    </row>
+    <row r="49" ht="18" customHeight="1">
+      <c r="B49" s="3" t="inlineStr">
+        <is>
+          <t>IPI:</t>
+        </is>
+      </c>
+      <c r="C49" s="32" t="n"/>
+      <c r="D49" s="99" t="n"/>
+      <c r="E49" s="99" t="n"/>
+      <c r="F49" s="99" t="n"/>
+      <c r="G49" s="99" t="n"/>
+      <c r="H49" s="99" t="n"/>
+      <c r="I49" s="99" t="n"/>
+      <c r="J49" s="101" t="n"/>
+    </row>
+    <row r="50" ht="18" customHeight="1">
+      <c r="B50" s="5" t="inlineStr">
+        <is>
+          <t>ICMS ORIGEM:</t>
+        </is>
+      </c>
+      <c r="C50" s="44" t="n"/>
+      <c r="D50" s="99" t="n"/>
+      <c r="E50" s="99" t="n"/>
+      <c r="F50" s="99" t="n"/>
+      <c r="G50" s="99" t="n"/>
+      <c r="H50" s="99" t="n"/>
+      <c r="I50" s="99" t="n"/>
+      <c r="J50" s="101" t="n"/>
+    </row>
+    <row r="51" ht="18" customHeight="1">
+      <c r="B51" s="3" t="inlineStr">
+        <is>
+          <t>ICMS ENTRADA (SAIDA FORNEDOR):</t>
+        </is>
+      </c>
+      <c r="C51" s="46" t="n"/>
+      <c r="D51" s="101" t="n"/>
+      <c r="E51" s="4" t="inlineStr">
+        <is>
+          <t>CST ICMS</t>
+        </is>
+      </c>
+      <c r="F51" s="47" t="n"/>
+      <c r="G51" s="99" t="n"/>
+      <c r="H51" s="99" t="n"/>
+      <c r="I51" s="99" t="n"/>
+      <c r="J51" s="101" t="n"/>
+    </row>
+    <row r="52" ht="18" customHeight="1">
+      <c r="B52" s="5" t="inlineStr">
+        <is>
+          <t>REDUÇÃO DE ICMS:</t>
+        </is>
+      </c>
+      <c r="C52" s="49" t="n"/>
+      <c r="D52" s="99" t="n"/>
+      <c r="E52" s="99" t="n"/>
+      <c r="F52" s="99" t="n"/>
+      <c r="G52" s="99" t="n"/>
+      <c r="H52" s="99" t="n"/>
+      <c r="I52" s="99" t="n"/>
+      <c r="J52" s="101" t="n"/>
+    </row>
+    <row r="53" ht="18" customHeight="1">
+      <c r="B53" s="3" t="inlineStr">
+        <is>
+          <t>IVA%</t>
+        </is>
+      </c>
+      <c r="C53" s="32" t="n"/>
+      <c r="D53" s="99" t="n"/>
+      <c r="E53" s="99" t="n"/>
+      <c r="F53" s="99" t="n"/>
+      <c r="G53" s="99" t="n"/>
+      <c r="H53" s="99" t="n"/>
+      <c r="I53" s="99" t="n"/>
+      <c r="J53" s="101" t="n"/>
+    </row>
+    <row r="54" ht="18" customHeight="1">
+      <c r="B54" s="5" t="inlineStr">
+        <is>
+          <t>PAUTA%</t>
+        </is>
+      </c>
+      <c r="C54" s="34" t="n"/>
+      <c r="D54" s="99" t="n"/>
+      <c r="E54" s="99" t="n"/>
+      <c r="F54" s="99" t="n"/>
+      <c r="G54" s="99" t="n"/>
+      <c r="H54" s="99" t="n"/>
+      <c r="I54" s="99" t="n"/>
+      <c r="J54" s="101" t="n"/>
+    </row>
+    <row r="55" ht="18" customHeight="1">
+      <c r="B55" s="3" t="inlineStr">
+        <is>
+          <t>PIS%</t>
+        </is>
+      </c>
+      <c r="C55" s="42" t="n"/>
+      <c r="D55" s="101" t="n"/>
+      <c r="E55" s="4" t="inlineStr">
+        <is>
+          <t>CST PIS</t>
+        </is>
+      </c>
+      <c r="F55" s="42" t="n"/>
+      <c r="G55" s="99" t="n"/>
+      <c r="H55" s="99" t="n"/>
+      <c r="I55" s="99" t="n"/>
+      <c r="J55" s="101" t="n"/>
+    </row>
+    <row r="56" ht="18" customHeight="1" thickBot="1">
+      <c r="B56" s="7" t="inlineStr">
+        <is>
+          <t>COFINS%:</t>
+        </is>
+      </c>
+      <c r="C56" s="36" t="n"/>
+      <c r="D56" s="107" t="n"/>
+      <c r="E56" s="8" t="inlineStr">
+        <is>
+          <t>CST COFINS</t>
+        </is>
+      </c>
+      <c r="F56" s="36" t="n"/>
+      <c r="G56" s="106" t="n"/>
+      <c r="H56" s="106" t="n"/>
+      <c r="I56" s="106" t="n"/>
+      <c r="J56" s="107" t="n"/>
+    </row>
+    <row r="57" ht="18" customHeight="1" thickBot="1"/>
+    <row r="58" ht="18" customHeight="1">
+      <c r="B58" s="38" t="inlineStr">
+        <is>
+          <t>INFORMAÇÕES PREENCHIDAS PELA COMERCIAL OSWALDO CRUZ</t>
+        </is>
+      </c>
+      <c r="C58" s="93" t="n"/>
+      <c r="D58" s="93" t="n"/>
+      <c r="E58" s="93" t="n"/>
+      <c r="F58" s="93" t="n"/>
+      <c r="G58" s="93" t="n"/>
+      <c r="H58" s="93" t="n"/>
+      <c r="I58" s="93" t="n"/>
+      <c r="J58" s="94" t="n"/>
+    </row>
+    <row r="59" ht="18" customHeight="1">
+      <c r="B59" s="5" t="inlineStr">
+        <is>
+          <t>COMPRADOR:</t>
+        </is>
+      </c>
+      <c r="C59" s="34" t="n"/>
+      <c r="D59" s="99" t="n"/>
+      <c r="E59" s="99" t="n"/>
+      <c r="F59" s="99" t="n"/>
+      <c r="G59" s="99" t="n"/>
+      <c r="H59" s="99" t="n"/>
+      <c r="I59" s="99" t="n"/>
+      <c r="J59" s="101" t="n"/>
+    </row>
+    <row r="60" ht="18" customFormat="1" customHeight="1" s="9">
+      <c r="B60" s="3" t="inlineStr">
+        <is>
+          <t>MAPA:</t>
+        </is>
+      </c>
+      <c r="C60" s="41" t="inlineStr">
+        <is>
+          <t>A GRANDE (  )</t>
+        </is>
+      </c>
+      <c r="D60" s="115" t="n"/>
+      <c r="E60" s="41" t="inlineStr">
+        <is>
+          <t>A PEQUENO (  )</t>
+        </is>
+      </c>
+      <c r="F60" s="115" t="n"/>
+      <c r="G60" s="41" t="inlineStr">
+        <is>
+          <t>C GRANDE (  )</t>
+        </is>
+      </c>
+      <c r="H60" s="115" t="n"/>
+      <c r="I60" s="41" t="inlineStr">
+        <is>
+          <t>C PEQUENO (  )</t>
+        </is>
+      </c>
+      <c r="J60" s="14" t="n"/>
+    </row>
+    <row r="61" ht="18" customFormat="1" customHeight="1" s="9">
+      <c r="B61" s="5" t="inlineStr">
+        <is>
+          <t>ESTOQUES MÍNIMO E MÁXIMO:</t>
+        </is>
+      </c>
+      <c r="C61" s="6" t="inlineStr">
+        <is>
+          <t>MÍN:</t>
+        </is>
+      </c>
+      <c r="D61" s="6" t="inlineStr">
+        <is>
+          <t>MÁX:</t>
+        </is>
+      </c>
+      <c r="E61" s="6" t="inlineStr">
+        <is>
+          <t>MÍN:</t>
+        </is>
+      </c>
+      <c r="F61" s="6" t="inlineStr">
+        <is>
+          <t>MÁX:</t>
+        </is>
+      </c>
+      <c r="G61" s="6" t="inlineStr">
+        <is>
+          <t>MÍN:</t>
+        </is>
+      </c>
+      <c r="H61" s="6" t="inlineStr">
+        <is>
+          <t>MÁX:</t>
+        </is>
+      </c>
+      <c r="I61" s="6" t="inlineStr">
+        <is>
+          <t>MÍN:</t>
+        </is>
+      </c>
+      <c r="J61" s="15" t="inlineStr">
+        <is>
+          <t>MÁX:</t>
+        </is>
+      </c>
+    </row>
+    <row r="62" ht="18" customHeight="1">
+      <c r="B62" s="3" t="inlineStr">
+        <is>
+          <t>DISTRIBUIDO POR:</t>
+        </is>
+      </c>
+      <c r="C62" s="4" t="inlineStr">
+        <is>
+          <t>MATRIZ (  )</t>
+        </is>
+      </c>
+      <c r="D62" s="4" t="inlineStr">
+        <is>
+          <t>LOJA 05 (  )</t>
+        </is>
+      </c>
+      <c r="E62" s="4" t="inlineStr">
+        <is>
+          <t>LOJA 07 (  )</t>
+        </is>
+      </c>
+      <c r="F62" s="4" t="inlineStr">
+        <is>
+          <t>LOJA 20 (  )</t>
+        </is>
+      </c>
+      <c r="G62" s="4" t="inlineStr">
+        <is>
+          <t>LOJA 11(  )</t>
+        </is>
+      </c>
+      <c r="H62" s="4" t="n"/>
+      <c r="I62" s="4" t="n"/>
+      <c r="J62" s="14" t="n"/>
+    </row>
+    <row r="63" ht="18" customHeight="1">
+      <c r="B63" s="5" t="inlineStr">
+        <is>
+          <t>FORMA DE ABASTECIMENTO:</t>
+        </is>
+      </c>
+      <c r="C63" s="30" t="inlineStr">
+        <is>
+          <t>CENTRAL - CENTRAL (  )</t>
+        </is>
+      </c>
+      <c r="D63" s="115" t="n"/>
+      <c r="E63" s="30" t="inlineStr">
+        <is>
+          <t>CENTRAL - LOJA (  )</t>
+        </is>
+      </c>
+      <c r="F63" s="115" t="n"/>
+      <c r="G63" s="30" t="inlineStr">
+        <is>
+          <t>LOJA - LOJA (  )</t>
+        </is>
+      </c>
+      <c r="H63" s="115" t="n"/>
+      <c r="I63" s="30" t="inlineStr">
+        <is>
+          <t>CROSSDOCKING (  )</t>
+        </is>
+      </c>
+      <c r="J63" s="115" t="n"/>
+    </row>
+    <row r="64" ht="18" customHeight="1">
+      <c r="B64" s="3" t="inlineStr">
+        <is>
+          <t>JÁ EXISTE FAMÍLIA CADASTRADA?</t>
+        </is>
+      </c>
+      <c r="C64" s="32" t="n"/>
+      <c r="D64" s="99" t="n"/>
+      <c r="E64" s="99" t="n"/>
+      <c r="F64" s="99" t="n"/>
+      <c r="G64" s="99" t="n"/>
+      <c r="H64" s="99" t="n"/>
+      <c r="I64" s="99" t="n"/>
+      <c r="J64" s="101" t="n"/>
+    </row>
+    <row r="65" ht="18" customHeight="1">
+      <c r="B65" s="5" t="inlineStr">
+        <is>
+          <t>INFORME O CÓDIGO DA FAMÍLIA:</t>
+        </is>
+      </c>
+      <c r="C65" s="34" t="n"/>
+      <c r="D65" s="99" t="n"/>
+      <c r="E65" s="99" t="n"/>
+      <c r="F65" s="99" t="n"/>
+      <c r="G65" s="99" t="n"/>
+      <c r="H65" s="99" t="n"/>
+      <c r="I65" s="99" t="n"/>
+      <c r="J65" s="101" t="n"/>
+    </row>
+    <row r="66" ht="18" customHeight="1" thickBot="1">
+      <c r="B66" s="7" t="inlineStr">
+        <is>
+          <t>SEGMENTAÇÃO:</t>
+        </is>
+      </c>
+      <c r="C66" s="25" t="n"/>
+      <c r="D66" s="106" t="n"/>
+      <c r="E66" s="106" t="n"/>
+      <c r="F66" s="106" t="n"/>
+      <c r="G66" s="106" t="n"/>
+      <c r="H66" s="106" t="n"/>
+      <c r="I66" s="106" t="n"/>
+      <c r="J66" s="107" t="n"/>
+    </row>
+    <row r="67" ht="18" customHeight="1" thickBot="1">
+      <c r="B67" s="9" t="n"/>
+      <c r="E67" s="9" t="n"/>
+      <c r="F67" s="10" t="n"/>
+      <c r="G67" s="10" t="n"/>
+      <c r="H67" s="10" t="n"/>
+      <c r="I67" s="10" t="n"/>
+    </row>
+    <row r="68" ht="18" customHeight="1" thickBot="1">
+      <c r="B68" s="116" t="inlineStr">
+        <is>
+          <t>ATENÇÃO: TODO PRODUTO NOVO PRECISA DE UMA DIVISÃO INICIAL FEITA PELO COMPRADOR</t>
+        </is>
+      </c>
+      <c r="C68" s="117" t="n"/>
+      <c r="D68" s="117" t="n"/>
+      <c r="E68" s="117" t="n"/>
+      <c r="F68" s="117" t="n"/>
+      <c r="G68" s="117" t="n"/>
+      <c r="H68" s="117" t="n"/>
+      <c r="I68" s="117" t="n"/>
+      <c r="J68" s="118" t="n"/>
+    </row>
+    <row r="69" ht="18" customHeight="1"/>
+    <row r="70" ht="18" customHeight="1"/>
+    <row r="71" ht="18" customHeight="1">
+      <c r="B71" s="16" t="inlineStr">
+        <is>
+          <t>DATA</t>
+        </is>
+      </c>
+      <c r="C71" s="9" t="n"/>
+      <c r="D71" s="16" t="inlineStr">
+        <is>
+          <t>COMPRADOR</t>
+        </is>
+      </c>
+      <c r="E71" s="16" t="n"/>
+      <c r="F71" s="9" t="n"/>
+      <c r="G71" s="9" t="n"/>
+      <c r="H71" s="16" t="inlineStr">
+        <is>
+          <t>GERENTE COMPRAS</t>
+        </is>
+      </c>
+      <c r="I71" s="16" t="n"/>
+      <c r="J71" s="9" t="n"/>
+    </row>
+  </sheetData>
+  <mergeCells count="87">
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C33:J33"/>
+    <mergeCell ref="F10:J10"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="F6:J6"/>
+    <mergeCell ref="C20:J20"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="E63:F63"/>
+    <mergeCell ref="F18:J18"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="F8:J8"/>
+    <mergeCell ref="F17:J17"/>
+    <mergeCell ref="C59:J59"/>
+    <mergeCell ref="C52:J52"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F9:J9"/>
+    <mergeCell ref="B25:J25"/>
+    <mergeCell ref="C48:J48"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="C32:J32"/>
+    <mergeCell ref="F7:J7"/>
+    <mergeCell ref="C26:J26"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="F51:J51"/>
+    <mergeCell ref="C16:J16"/>
+    <mergeCell ref="C50:J50"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="B15:J15"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C28:J28"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="G60:H60"/>
+    <mergeCell ref="B58:J58"/>
+    <mergeCell ref="C30:J30"/>
+    <mergeCell ref="B42:J42"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="C64:J64"/>
+    <mergeCell ref="F55:J55"/>
+    <mergeCell ref="F12:J12"/>
+    <mergeCell ref="B35:J36"/>
+    <mergeCell ref="C54:J54"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C43:J43"/>
+    <mergeCell ref="F23:J23"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C27:J27"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="B46:J46"/>
+    <mergeCell ref="G63:H63"/>
+    <mergeCell ref="I63:J63"/>
+    <mergeCell ref="C66:J66"/>
+    <mergeCell ref="C19:J19"/>
+    <mergeCell ref="C53:J53"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C29:J29"/>
+    <mergeCell ref="C65:J65"/>
+    <mergeCell ref="C47:J47"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C44:J44"/>
+    <mergeCell ref="C22:J22"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="C31:J31"/>
+    <mergeCell ref="B68:J68"/>
+    <mergeCell ref="C21:J21"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="F13:J13"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="F56:J56"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="C49:J49"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
+  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B1:N71"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="1.5703125" customWidth="1" style="1" min="1" max="1"/>
+    <col width="33.28515625" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
+    <col width="15.7109375" customWidth="1" style="1" min="3" max="3"/>
+    <col width="14.7109375" customWidth="1" style="1" min="4" max="4"/>
+    <col width="23.7109375" customWidth="1" style="1" min="5" max="5"/>
+    <col width="14.7109375" customWidth="1" style="1" min="6" max="9"/>
+    <col width="11.5703125" customWidth="1" style="1" min="10" max="10"/>
+    <col width="9.140625" customWidth="1" style="1" min="11" max="16384"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="44.25" customHeight="1" thickBot="1">
+      <c r="B1" s="90" t="inlineStr">
+        <is>
+          <t>CADASTRO SUPERMERCADOS JOANIN LTDA</t>
+        </is>
+      </c>
+      <c r="C1" s="91" t="n"/>
+      <c r="D1" s="91" t="n"/>
+      <c r="E1" s="91" t="n"/>
+      <c r="F1" s="91" t="n"/>
+      <c r="G1" s="91" t="n"/>
+      <c r="H1" s="91" t="n"/>
+      <c r="I1" s="91" t="n"/>
+      <c r="J1" s="92" t="n"/>
+    </row>
+    <row r="2" ht="18" customHeight="1" thickBot="1"/>
+    <row r="3" ht="18" customHeight="1">
+      <c r="B3" s="38" t="inlineStr">
+        <is>
+          <t>INFORMAÇÕES FORNECEDOR</t>
+        </is>
+      </c>
+      <c r="C3" s="93" t="n"/>
+      <c r="D3" s="93" t="n"/>
+      <c r="E3" s="93" t="n"/>
+      <c r="F3" s="93" t="n"/>
+      <c r="G3" s="93" t="n"/>
+      <c r="H3" s="93" t="n"/>
+      <c r="I3" s="93" t="n"/>
+      <c r="J3" s="94" t="n"/>
+    </row>
+    <row r="4" ht="18" customHeight="1">
+      <c r="B4" s="95" t="inlineStr">
+        <is>
+          <t>É FORNECEDOR NOVO (    ) SIM     (   ) NÃO                           -                            FOI FEITO CONTRATO (   ) SIM      (    ) NÃO</t>
+        </is>
+      </c>
+      <c r="C4" s="96" t="n"/>
+      <c r="D4" s="96" t="n"/>
+      <c r="E4" s="96" t="n"/>
+      <c r="F4" s="96" t="n"/>
+      <c r="G4" s="96" t="n"/>
+      <c r="H4" s="96" t="n"/>
+      <c r="I4" s="96" t="n"/>
+      <c r="J4" s="97" t="n"/>
+    </row>
+    <row r="5" ht="18" customHeight="1">
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>RAZÃO SOCIAL:</t>
+        </is>
+      </c>
+      <c r="C5" s="98" t="inlineStr">
+        <is>
+          <t>NETFEIRA PONTOCOM LTDA</t>
+        </is>
+      </c>
+      <c r="D5" s="99" t="n"/>
+      <c r="E5" s="99" t="n"/>
+      <c r="F5" s="99" t="n"/>
+      <c r="G5" s="99" t="n"/>
+      <c r="H5" s="99" t="n"/>
+      <c r="I5" s="99" t="n"/>
+      <c r="J5" s="100" t="n"/>
+    </row>
+    <row r="6" ht="18" customHeight="1">
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+      <c r="C6" s="51" t="inlineStr">
+        <is>
+          <t>03.974.724/0001-24</t>
+        </is>
+      </c>
+      <c r="D6" s="101" t="n"/>
+      <c r="E6" s="4" t="inlineStr">
+        <is>
+          <t>INSC. ESTADUAL:</t>
+        </is>
+      </c>
+      <c r="F6" s="72" t="inlineStr">
+        <is>
+          <t>115.951.284-113</t>
+        </is>
+      </c>
+      <c r="G6" s="99" t="n"/>
+      <c r="H6" s="99" t="n"/>
+      <c r="I6" s="99" t="n"/>
+      <c r="J6" s="101" t="n"/>
+    </row>
+    <row r="7" ht="18" customHeight="1">
+      <c r="B7" s="5" t="inlineStr">
+        <is>
+          <t>ENDEREÇO:</t>
+        </is>
+      </c>
+      <c r="C7" s="71" t="inlineStr">
+        <is>
+          <t>AVENIDA DOUTOR GASTÃO VIDIGAL</t>
+        </is>
+      </c>
+      <c r="D7" s="101" t="n"/>
+      <c r="E7" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nº </t>
+        </is>
+      </c>
+      <c r="F7" s="72" t="inlineStr">
+        <is>
+          <t>1946</t>
+        </is>
+      </c>
+      <c r="G7" s="99" t="n"/>
+      <c r="H7" s="99" t="n"/>
+      <c r="I7" s="99" t="n"/>
+      <c r="J7" s="101" t="n"/>
+    </row>
+    <row r="8" ht="18" customHeight="1">
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BAIRRO: </t>
+        </is>
+      </c>
+      <c r="C8" s="51" t="inlineStr">
+        <is>
+          <t>VILA LEOPOLDINA</t>
+        </is>
+      </c>
+      <c r="D8" s="101" t="n"/>
+      <c r="E8" s="4" t="inlineStr">
+        <is>
+          <t>CEP:</t>
+        </is>
+      </c>
+      <c r="F8" s="72" t="inlineStr">
+        <is>
+          <t>5316900</t>
+        </is>
+      </c>
+      <c r="G8" s="99" t="n"/>
+      <c r="H8" s="99" t="n"/>
+      <c r="I8" s="99" t="n"/>
+      <c r="J8" s="101" t="n"/>
+    </row>
+    <row r="9" ht="18" customHeight="1">
+      <c r="B9" s="5" t="inlineStr">
+        <is>
+          <t>CIDADE:</t>
+        </is>
+      </c>
+      <c r="C9" s="34" t="inlineStr">
+        <is>
+          <t>SÃO PAULO</t>
+        </is>
+      </c>
+      <c r="D9" s="101" t="n"/>
+      <c r="E9" s="6" t="inlineStr">
+        <is>
+          <t>ESTADO:</t>
+        </is>
+      </c>
+      <c r="F9" s="71" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="G9" s="99" t="n"/>
+      <c r="H9" s="99" t="n"/>
+      <c r="I9" s="99" t="n"/>
+      <c r="J9" s="101" t="n"/>
+    </row>
+    <row r="10" ht="18" customHeight="1">
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>COMPLEMENTO:</t>
+        </is>
+      </c>
+      <c r="C10" s="51" t="inlineStr">
+        <is>
+          <t>P.AMA BOX 61/62,AMB BOX 3,4</t>
+        </is>
+      </c>
+      <c r="D10" s="101" t="n"/>
+      <c r="E10" s="19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PRAZO DE PGTO </t>
+        </is>
+      </c>
+      <c r="F10" s="102" t="n"/>
+      <c r="G10" s="99" t="n"/>
+      <c r="H10" s="99" t="n"/>
+      <c r="I10" s="99" t="n"/>
+      <c r="J10" s="100" t="n"/>
+    </row>
+    <row r="11" ht="18" customHeight="1">
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>CONTATO :</t>
+        </is>
+      </c>
+      <c r="C11" s="51" t="n"/>
+      <c r="D11" s="101" t="n"/>
+      <c r="E11" s="4" t="inlineStr">
+        <is>
+          <t>TELEFONE :</t>
+        </is>
+      </c>
+      <c r="F11" s="75" t="n"/>
+      <c r="G11" s="76" t="n"/>
+      <c r="H11" s="76" t="n"/>
+      <c r="I11" s="76" t="n"/>
+      <c r="J11" s="77" t="n"/>
+    </row>
+    <row r="12" ht="18" customHeight="1">
+      <c r="B12" s="23" t="inlineStr">
+        <is>
+          <t>E-MAIL PARA ENVIO XML</t>
+        </is>
+      </c>
+      <c r="C12" s="78" t="n"/>
+      <c r="D12" s="101" t="n"/>
+      <c r="E12" s="24" t="inlineStr">
+        <is>
+          <t>E-MAIL PARA FINANCEIRO</t>
+        </is>
+      </c>
+      <c r="F12" s="80" t="n"/>
+      <c r="G12" s="99" t="n"/>
+      <c r="H12" s="99" t="n"/>
+      <c r="I12" s="99" t="n"/>
+      <c r="J12" s="101" t="n"/>
+    </row>
+    <row r="13" ht="18" customHeight="1" thickBot="1">
+      <c r="B13" s="67" t="inlineStr">
+        <is>
+          <t>(    )COM INDENIZAÇÃO - FORNECEDOR ACEITA NOTA FISCAL DE DEVOLUÇÃO</t>
+        </is>
+      </c>
+      <c r="C13" s="103" t="n"/>
+      <c r="D13" s="103" t="n"/>
+      <c r="E13" s="103" t="n"/>
+      <c r="F13" s="70" t="inlineStr">
+        <is>
+          <t>(    ) SEM INDENIZAÇÃO  -  FORNECEDOR NÃO ACEITA NOTA FISCAL DEVOLUÇÃO</t>
+        </is>
+      </c>
+      <c r="G13" s="104" t="n"/>
+      <c r="H13" s="104" t="n"/>
+      <c r="I13" s="104" t="n"/>
+      <c r="J13" s="105" t="n"/>
+    </row>
+    <row r="14" ht="18" customHeight="1" thickBot="1">
+      <c r="B14" s="9" t="n"/>
+      <c r="E14" s="9" t="n"/>
+      <c r="F14" s="10" t="n"/>
+      <c r="G14" s="10" t="n"/>
+      <c r="H14" s="10" t="n"/>
+      <c r="I14" s="10" t="n"/>
+    </row>
+    <row r="15" ht="18" customHeight="1">
+      <c r="B15" s="38" t="inlineStr">
+        <is>
+          <t>DADOS DO PRODUTO - UNIDADE</t>
+        </is>
+      </c>
+      <c r="C15" s="93" t="n"/>
+      <c r="D15" s="93" t="n"/>
+      <c r="E15" s="93" t="n"/>
+      <c r="F15" s="93" t="n"/>
+      <c r="G15" s="93" t="n"/>
+      <c r="H15" s="93" t="n"/>
+      <c r="I15" s="93" t="n"/>
+      <c r="J15" s="94" t="n"/>
+    </row>
+    <row r="16" ht="18" customHeight="1">
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t>DESCRIÇÃO:</t>
+        </is>
+      </c>
+      <c r="C16" s="32" t="inlineStr">
+        <is>
+          <t>AÇAI BUFALO COM MORANGO CONGELADO 1,300KG</t>
+        </is>
+      </c>
+      <c r="D16" s="99" t="n"/>
+      <c r="E16" s="99" t="n"/>
+      <c r="F16" s="99" t="n"/>
+      <c r="G16" s="99" t="n"/>
+      <c r="H16" s="99" t="n"/>
+      <c r="I16" s="99" t="n"/>
+      <c r="J16" s="101" t="n"/>
+      <c r="N16" s="11" t="n"/>
+    </row>
+    <row r="17" ht="18" customHeight="1">
+      <c r="B17" s="5" t="inlineStr">
+        <is>
+          <t>CÓD DE BARRAS:</t>
+        </is>
+      </c>
+      <c r="C17" s="65" t="inlineStr">
+        <is>
+          <t>7896519298655</t>
+        </is>
+      </c>
+      <c r="D17" s="101" t="n"/>
+      <c r="E17" s="12" t="inlineStr">
+        <is>
+          <t>MARCA:</t>
+        </is>
+      </c>
+      <c r="F17" s="65" t="inlineStr">
+        <is>
+          <t>DE MARCHI</t>
+        </is>
+      </c>
+      <c r="G17" s="99" t="n"/>
+      <c r="H17" s="99" t="n"/>
+      <c r="I17" s="99" t="n"/>
+      <c r="J17" s="101" t="n"/>
+    </row>
+    <row r="18" ht="18" customHeight="1">
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>PESO LIQUIDO KG:</t>
+        </is>
+      </c>
+      <c r="C18" s="51" t="inlineStr">
+        <is>
+          <t>1.3</t>
+        </is>
+      </c>
+      <c r="D18" s="101" t="n"/>
+      <c r="E18" s="4" t="inlineStr">
+        <is>
+          <t>PESO BRUTO KG:</t>
+        </is>
+      </c>
+      <c r="F18" s="32" t="inlineStr">
+        <is>
+          <t>1.3</t>
+        </is>
+      </c>
+      <c r="G18" s="99" t="n"/>
+      <c r="H18" s="99" t="n"/>
+      <c r="I18" s="99" t="n"/>
+      <c r="J18" s="101" t="n"/>
+    </row>
+    <row r="19" ht="18" customHeight="1">
+      <c r="B19" s="5" t="inlineStr">
+        <is>
+          <t>COMPRIMENTO EM CM:</t>
+        </is>
+      </c>
+      <c r="C19" s="34" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D19" s="99" t="n"/>
+      <c r="E19" s="99" t="n"/>
+      <c r="F19" s="99" t="n"/>
+      <c r="G19" s="99" t="n"/>
+      <c r="H19" s="99" t="n"/>
+      <c r="I19" s="99" t="n"/>
+      <c r="J19" s="101" t="n"/>
+    </row>
+    <row r="20" ht="18" customHeight="1">
+      <c r="B20" s="3" t="inlineStr">
+        <is>
+          <t>LARGURA EM CM:</t>
+        </is>
+      </c>
+      <c r="C20" s="57" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D20" s="99" t="n"/>
+      <c r="E20" s="99" t="n"/>
+      <c r="F20" s="99" t="n"/>
+      <c r="G20" s="99" t="n"/>
+      <c r="H20" s="99" t="n"/>
+      <c r="I20" s="99" t="n"/>
+      <c r="J20" s="101" t="n"/>
+    </row>
+    <row r="21" ht="18" customHeight="1">
+      <c r="B21" s="5" t="inlineStr">
+        <is>
+          <t>ALTURA EM CM:</t>
+        </is>
+      </c>
+      <c r="C21" s="59" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D21" s="99" t="n"/>
+      <c r="E21" s="99" t="n"/>
+      <c r="F21" s="99" t="n"/>
+      <c r="G21" s="99" t="n"/>
+      <c r="H21" s="99" t="n"/>
+      <c r="I21" s="99" t="n"/>
+      <c r="J21" s="101" t="n"/>
+    </row>
+    <row r="22" ht="18" customHeight="1">
+      <c r="B22" s="3" t="inlineStr">
+        <is>
+          <t>VALIDADE EM DIAS:</t>
+        </is>
+      </c>
+      <c r="C22" s="32" t="n"/>
+      <c r="D22" s="99" t="n"/>
+      <c r="E22" s="99" t="n"/>
+      <c r="F22" s="99" t="n"/>
+      <c r="G22" s="99" t="n"/>
+      <c r="H22" s="99" t="n"/>
+      <c r="I22" s="99" t="n"/>
+      <c r="J22" s="101" t="n"/>
+    </row>
+    <row r="23" ht="18" customHeight="1" thickBot="1">
+      <c r="B23" s="7" t="inlineStr">
+        <is>
+          <t>COD PRODUTO FORNECEDOR:</t>
+        </is>
+      </c>
+      <c r="C23" s="25" t="inlineStr">
+        <is>
+          <t>9633</t>
+        </is>
+      </c>
+      <c r="D23" s="106" t="n"/>
+      <c r="E23" s="107" t="n"/>
+      <c r="F23" s="61" t="inlineStr">
+        <is>
+          <t>(É OBRIGADOTÓRIO QUE O CÓDIGO DO FORNECEDOR SEJA O MESMO DO XML)</t>
+        </is>
+      </c>
+      <c r="G23" s="106" t="n"/>
+      <c r="H23" s="106" t="n"/>
+      <c r="I23" s="106" t="n"/>
+      <c r="J23" s="107" t="n"/>
+    </row>
+    <row r="24" ht="18" customHeight="1" thickBot="1"/>
+    <row r="25" ht="18" customHeight="1">
+      <c r="B25" s="38" t="inlineStr">
+        <is>
+          <t>DADOS DO PRODUTO - CAIXA</t>
+        </is>
+      </c>
+      <c r="C25" s="93" t="n"/>
+      <c r="D25" s="93" t="n"/>
+      <c r="E25" s="93" t="n"/>
+      <c r="F25" s="93" t="n"/>
+      <c r="G25" s="93" t="n"/>
+      <c r="H25" s="93" t="n"/>
+      <c r="I25" s="93" t="n"/>
+      <c r="J25" s="94" t="n"/>
+    </row>
+    <row r="26" ht="18" customHeight="1">
+      <c r="B26" s="3" t="inlineStr">
+        <is>
+          <t>TIPO DE EMBALAGEM:</t>
+        </is>
+      </c>
+      <c r="C26" s="32" t="inlineStr">
+        <is>
+          <t>UN</t>
+        </is>
+      </c>
+      <c r="D26" s="99" t="n"/>
+      <c r="E26" s="99" t="n"/>
+      <c r="F26" s="99" t="n"/>
+      <c r="G26" s="99" t="n"/>
+      <c r="H26" s="99" t="n"/>
+      <c r="I26" s="99" t="n"/>
+      <c r="J26" s="101" t="n"/>
+    </row>
+    <row r="27" ht="18" customHeight="1">
+      <c r="B27" s="5" t="inlineStr">
+        <is>
+          <t>QUANTIDADE NA CAIXA:</t>
+        </is>
+      </c>
+      <c r="C27" s="34" t="inlineStr">
+        <is>
+          <t>6.0</t>
+        </is>
+      </c>
+      <c r="D27" s="99" t="n"/>
+      <c r="E27" s="99" t="n"/>
+      <c r="F27" s="99" t="n"/>
+      <c r="G27" s="99" t="n"/>
+      <c r="H27" s="99" t="n"/>
+      <c r="I27" s="99" t="n"/>
+      <c r="J27" s="101" t="n"/>
+    </row>
+    <row r="28" ht="18" customHeight="1">
+      <c r="B28" s="3" t="inlineStr">
+        <is>
+          <t>CÓD DUN:</t>
+        </is>
+      </c>
+      <c r="C28" s="63" t="inlineStr">
+        <is>
+          <t>67896519298657</t>
+        </is>
+      </c>
+      <c r="D28" s="99" t="n"/>
+      <c r="E28" s="99" t="n"/>
+      <c r="F28" s="99" t="n"/>
+      <c r="G28" s="99" t="n"/>
+      <c r="H28" s="99" t="n"/>
+      <c r="I28" s="99" t="n"/>
+      <c r="J28" s="101" t="n"/>
+    </row>
+    <row r="29" ht="18" customHeight="1">
+      <c r="B29" s="5" t="inlineStr">
+        <is>
+          <t>PESO BRUTO KG:</t>
+        </is>
+      </c>
+      <c r="C29" s="34" t="inlineStr">
+        <is>
+          <t>7.8</t>
+        </is>
+      </c>
+      <c r="D29" s="99" t="n"/>
+      <c r="E29" s="99" t="n"/>
+      <c r="F29" s="99" t="n"/>
+      <c r="G29" s="99" t="n"/>
+      <c r="H29" s="99" t="n"/>
+      <c r="I29" s="99" t="n"/>
+      <c r="J29" s="101" t="n"/>
+    </row>
+    <row r="30" ht="18" customHeight="1">
+      <c r="B30" s="3" t="inlineStr">
+        <is>
+          <t>PESO LIQUIDO KG:</t>
+        </is>
+      </c>
+      <c r="C30" s="32" t="inlineStr">
+        <is>
+          <t>7.8</t>
+        </is>
+      </c>
+      <c r="D30" s="99" t="n"/>
+      <c r="E30" s="99" t="n"/>
+      <c r="F30" s="99" t="n"/>
+      <c r="G30" s="99" t="n"/>
+      <c r="H30" s="99" t="n"/>
+      <c r="I30" s="99" t="n"/>
+      <c r="J30" s="101" t="n"/>
+    </row>
+    <row r="31" ht="18" customHeight="1">
+      <c r="B31" s="5" t="inlineStr">
+        <is>
+          <t>COMPRIMENTO EM CM:</t>
+        </is>
+      </c>
+      <c r="C31" s="34" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D31" s="99" t="n"/>
+      <c r="E31" s="99" t="n"/>
+      <c r="F31" s="99" t="n"/>
+      <c r="G31" s="99" t="n"/>
+      <c r="H31" s="99" t="n"/>
+      <c r="I31" s="99" t="n"/>
+      <c r="J31" s="101" t="n"/>
+    </row>
+    <row r="32" ht="18" customHeight="1">
+      <c r="B32" s="3" t="inlineStr">
+        <is>
+          <t>LARGURA EM CM:</t>
+        </is>
+      </c>
+      <c r="C32" s="32" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D32" s="99" t="n"/>
+      <c r="E32" s="99" t="n"/>
+      <c r="F32" s="99" t="n"/>
+      <c r="G32" s="99" t="n"/>
+      <c r="H32" s="99" t="n"/>
+      <c r="I32" s="99" t="n"/>
+      <c r="J32" s="101" t="n"/>
+    </row>
+    <row r="33" ht="18" customHeight="1" thickBot="1">
+      <c r="B33" s="7" t="inlineStr">
+        <is>
+          <t>ALTURA EM CM:</t>
+        </is>
+      </c>
+      <c r="C33" s="25" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D33" s="106" t="n"/>
+      <c r="E33" s="106" t="n"/>
+      <c r="F33" s="106" t="n"/>
+      <c r="G33" s="106" t="n"/>
+      <c r="H33" s="106" t="n"/>
+      <c r="I33" s="106" t="n"/>
+      <c r="J33" s="107" t="n"/>
+    </row>
+    <row r="34" ht="18" customHeight="1" thickBot="1"/>
+    <row r="35" ht="18" customHeight="1">
+      <c r="B35" s="38" t="inlineStr">
+        <is>
+          <t>CUSTO DO PRODUTO - UNITÁRIO</t>
+        </is>
+      </c>
+      <c r="C35" s="108" t="n"/>
+      <c r="D35" s="108" t="n"/>
+      <c r="E35" s="108" t="n"/>
+      <c r="F35" s="108" t="n"/>
+      <c r="G35" s="108" t="n"/>
+      <c r="H35" s="108" t="n"/>
+      <c r="I35" s="108" t="n"/>
+      <c r="J35" s="109" t="n"/>
+    </row>
+    <row r="36" ht="18" customHeight="1">
+      <c r="B36" s="110" t="n"/>
+      <c r="C36" s="111" t="n"/>
+      <c r="D36" s="111" t="n"/>
+      <c r="E36" s="111" t="n"/>
+      <c r="F36" s="111" t="n"/>
+      <c r="G36" s="111" t="n"/>
+      <c r="H36" s="111" t="n"/>
+      <c r="I36" s="111" t="n"/>
+      <c r="J36" s="112" t="n"/>
+    </row>
+    <row r="37" ht="18" customHeight="1">
+      <c r="B37" s="17" t="inlineStr">
+        <is>
+          <t>CUSTO SEM ST:</t>
+        </is>
+      </c>
+      <c r="C37" s="51" t="n"/>
+      <c r="D37" s="101" t="n"/>
+      <c r="E37" s="52" t="inlineStr">
+        <is>
+          <t>CUSTO COM ST:</t>
+        </is>
+      </c>
+      <c r="F37" s="113" t="n"/>
+      <c r="G37" s="51" t="n"/>
+      <c r="H37" s="101" t="n"/>
+      <c r="I37" s="52" t="n"/>
+      <c r="J37" s="113" t="n"/>
+    </row>
+    <row r="38" ht="18" customHeight="1">
+      <c r="B38" s="17" t="inlineStr">
+        <is>
+          <t>VALOR DA ST:</t>
+        </is>
+      </c>
+      <c r="C38" s="51" t="n"/>
+      <c r="D38" s="101" t="n"/>
+      <c r="E38" s="52" t="inlineStr">
+        <is>
+          <t>CUSTO UNITÁRIO FINAL:</t>
+        </is>
+      </c>
+      <c r="F38" s="113" t="n"/>
+      <c r="G38" s="51" t="n"/>
+      <c r="H38" s="101" t="n"/>
+      <c r="I38" s="52" t="n"/>
+      <c r="J38" s="113" t="n"/>
+    </row>
+    <row r="39" ht="18" customHeight="1">
+      <c r="B39" s="17" t="inlineStr">
+        <is>
+          <t>VERBA:</t>
+        </is>
+      </c>
+      <c r="C39" s="51" t="n"/>
+      <c r="D39" s="101" t="n"/>
+      <c r="E39" s="52" t="inlineStr">
+        <is>
+          <t>MARGEM:</t>
+        </is>
+      </c>
+      <c r="F39" s="113" t="n"/>
+      <c r="G39" s="51" t="n"/>
+      <c r="H39" s="101" t="n"/>
+      <c r="I39" s="52" t="n"/>
+      <c r="J39" s="113" t="n"/>
+    </row>
+    <row r="40" ht="18" customHeight="1" thickBot="1">
+      <c r="B40" s="18" t="n"/>
+      <c r="C40" s="53" t="n"/>
+      <c r="D40" s="107" t="n"/>
+      <c r="E40" s="54" t="inlineStr">
+        <is>
+          <t>VALOR DE VENDA:</t>
+        </is>
+      </c>
+      <c r="F40" s="114" t="n"/>
+      <c r="G40" s="53" t="n"/>
+      <c r="H40" s="107" t="n"/>
+      <c r="I40" s="54" t="n"/>
+      <c r="J40" s="114" t="n"/>
+    </row>
+    <row r="41" ht="18" customHeight="1" thickBot="1"/>
+    <row r="42" ht="18" customHeight="1">
+      <c r="B42" s="38" t="inlineStr">
+        <is>
+          <t>DADOS PALLETIZAÇÃO</t>
+        </is>
+      </c>
+      <c r="C42" s="93" t="n"/>
+      <c r="D42" s="93" t="n"/>
+      <c r="E42" s="93" t="n"/>
+      <c r="F42" s="93" t="n"/>
+      <c r="G42" s="93" t="n"/>
+      <c r="H42" s="93" t="n"/>
+      <c r="I42" s="93" t="n"/>
+      <c r="J42" s="94" t="n"/>
+    </row>
+    <row r="43" ht="18" customHeight="1">
+      <c r="B43" s="3" t="inlineStr">
+        <is>
+          <t>LASTRO/CAMADA:</t>
+        </is>
+      </c>
+      <c r="C43" s="32" t="n"/>
+      <c r="D43" s="99" t="n"/>
+      <c r="E43" s="99" t="n"/>
+      <c r="F43" s="99" t="n"/>
+      <c r="G43" s="99" t="n"/>
+      <c r="H43" s="99" t="n"/>
+      <c r="I43" s="99" t="n"/>
+      <c r="J43" s="101" t="n"/>
+    </row>
+    <row r="44" ht="18" customHeight="1" thickBot="1">
+      <c r="B44" s="7" t="inlineStr">
+        <is>
+          <t>ALTURA:</t>
+        </is>
+      </c>
+      <c r="C44" s="25" t="n"/>
+      <c r="D44" s="106" t="n"/>
+      <c r="E44" s="106" t="n"/>
+      <c r="F44" s="106" t="n"/>
+      <c r="G44" s="106" t="n"/>
+      <c r="H44" s="106" t="n"/>
+      <c r="I44" s="106" t="n"/>
+      <c r="J44" s="107" t="n"/>
+    </row>
+    <row r="45" ht="18" customHeight="1" thickBot="1"/>
+    <row r="46" ht="18" customHeight="1">
+      <c r="B46" s="38" t="inlineStr">
+        <is>
+          <t>INFORMAÇÕES FISCAIS</t>
+        </is>
+      </c>
+      <c r="C46" s="93" t="n"/>
+      <c r="D46" s="93" t="n"/>
+      <c r="E46" s="93" t="n"/>
+      <c r="F46" s="93" t="n"/>
+      <c r="G46" s="93" t="n"/>
+      <c r="H46" s="93" t="n"/>
+      <c r="I46" s="93" t="n"/>
+      <c r="J46" s="94" t="n"/>
+    </row>
+    <row r="47" ht="18" customHeight="1">
+      <c r="B47" s="3" t="inlineStr">
+        <is>
+          <t>NCM:</t>
+        </is>
+      </c>
+      <c r="C47" s="32" t="inlineStr">
+        <is>
+          <t>2106.90.90</t>
+        </is>
+      </c>
+      <c r="D47" s="99" t="n"/>
+      <c r="E47" s="99" t="n"/>
+      <c r="F47" s="99" t="n"/>
+      <c r="G47" s="99" t="n"/>
+      <c r="H47" s="99" t="n"/>
+      <c r="I47" s="99" t="n"/>
+      <c r="J47" s="101" t="n"/>
+    </row>
+    <row r="48" ht="18" customHeight="1">
+      <c r="B48" s="5" t="inlineStr">
+        <is>
+          <t>CEST:</t>
+        </is>
+      </c>
+      <c r="C48" s="34" t="inlineStr">
+        <is>
+          <t>020</t>
+        </is>
+      </c>
+      <c r="D48" s="99" t="n"/>
+      <c r="E48" s="99" t="n"/>
+      <c r="F48" s="99" t="n"/>
+      <c r="G48" s="99" t="n"/>
+      <c r="H48" s="99" t="n"/>
+      <c r="I48" s="99" t="n"/>
+      <c r="J48" s="101" t="n"/>
+    </row>
+    <row r="49" ht="18" customHeight="1">
+      <c r="B49" s="3" t="inlineStr">
+        <is>
+          <t>IPI:</t>
+        </is>
+      </c>
+      <c r="C49" s="32" t="n"/>
+      <c r="D49" s="99" t="n"/>
+      <c r="E49" s="99" t="n"/>
+      <c r="F49" s="99" t="n"/>
+      <c r="G49" s="99" t="n"/>
+      <c r="H49" s="99" t="n"/>
+      <c r="I49" s="99" t="n"/>
+      <c r="J49" s="101" t="n"/>
+    </row>
+    <row r="50" ht="18" customHeight="1">
+      <c r="B50" s="5" t="inlineStr">
+        <is>
+          <t>ICMS ORIGEM:</t>
+        </is>
+      </c>
+      <c r="C50" s="44" t="n"/>
+      <c r="D50" s="99" t="n"/>
+      <c r="E50" s="99" t="n"/>
+      <c r="F50" s="99" t="n"/>
+      <c r="G50" s="99" t="n"/>
+      <c r="H50" s="99" t="n"/>
+      <c r="I50" s="99" t="n"/>
+      <c r="J50" s="101" t="n"/>
+    </row>
+    <row r="51" ht="18" customHeight="1">
+      <c r="B51" s="3" t="inlineStr">
+        <is>
+          <t>ICMS ENTRADA (SAIDA FORNEDOR):</t>
+        </is>
+      </c>
+      <c r="C51" s="46" t="n"/>
+      <c r="D51" s="101" t="n"/>
+      <c r="E51" s="4" t="inlineStr">
+        <is>
+          <t>CST ICMS</t>
+        </is>
+      </c>
+      <c r="F51" s="47" t="n"/>
+      <c r="G51" s="99" t="n"/>
+      <c r="H51" s="99" t="n"/>
+      <c r="I51" s="99" t="n"/>
+      <c r="J51" s="101" t="n"/>
+    </row>
+    <row r="52" ht="18" customHeight="1">
+      <c r="B52" s="5" t="inlineStr">
+        <is>
+          <t>REDUÇÃO DE ICMS:</t>
+        </is>
+      </c>
+      <c r="C52" s="49" t="n"/>
+      <c r="D52" s="99" t="n"/>
+      <c r="E52" s="99" t="n"/>
+      <c r="F52" s="99" t="n"/>
+      <c r="G52" s="99" t="n"/>
+      <c r="H52" s="99" t="n"/>
+      <c r="I52" s="99" t="n"/>
+      <c r="J52" s="101" t="n"/>
+    </row>
+    <row r="53" ht="18" customHeight="1">
+      <c r="B53" s="3" t="inlineStr">
+        <is>
+          <t>IVA%</t>
+        </is>
+      </c>
+      <c r="C53" s="32" t="n"/>
+      <c r="D53" s="99" t="n"/>
+      <c r="E53" s="99" t="n"/>
+      <c r="F53" s="99" t="n"/>
+      <c r="G53" s="99" t="n"/>
+      <c r="H53" s="99" t="n"/>
+      <c r="I53" s="99" t="n"/>
+      <c r="J53" s="101" t="n"/>
+    </row>
+    <row r="54" ht="18" customHeight="1">
+      <c r="B54" s="5" t="inlineStr">
+        <is>
+          <t>PAUTA%</t>
+        </is>
+      </c>
+      <c r="C54" s="34" t="n"/>
+      <c r="D54" s="99" t="n"/>
+      <c r="E54" s="99" t="n"/>
+      <c r="F54" s="99" t="n"/>
+      <c r="G54" s="99" t="n"/>
+      <c r="H54" s="99" t="n"/>
+      <c r="I54" s="99" t="n"/>
+      <c r="J54" s="101" t="n"/>
+    </row>
+    <row r="55" ht="18" customHeight="1">
+      <c r="B55" s="3" t="inlineStr">
+        <is>
+          <t>PIS%</t>
+        </is>
+      </c>
+      <c r="C55" s="42" t="n"/>
+      <c r="D55" s="101" t="n"/>
+      <c r="E55" s="4" t="inlineStr">
+        <is>
+          <t>CST PIS</t>
+        </is>
+      </c>
+      <c r="F55" s="42" t="n"/>
+      <c r="G55" s="99" t="n"/>
+      <c r="H55" s="99" t="n"/>
+      <c r="I55" s="99" t="n"/>
+      <c r="J55" s="101" t="n"/>
+    </row>
+    <row r="56" ht="18" customHeight="1" thickBot="1">
+      <c r="B56" s="7" t="inlineStr">
+        <is>
+          <t>COFINS%:</t>
+        </is>
+      </c>
+      <c r="C56" s="36" t="n"/>
+      <c r="D56" s="107" t="n"/>
+      <c r="E56" s="8" t="inlineStr">
+        <is>
+          <t>CST COFINS</t>
+        </is>
+      </c>
+      <c r="F56" s="36" t="n"/>
+      <c r="G56" s="106" t="n"/>
+      <c r="H56" s="106" t="n"/>
+      <c r="I56" s="106" t="n"/>
+      <c r="J56" s="107" t="n"/>
+    </row>
+    <row r="57" ht="18" customHeight="1" thickBot="1"/>
+    <row r="58" ht="18" customHeight="1">
+      <c r="B58" s="38" t="inlineStr">
+        <is>
+          <t>INFORMAÇÕES PREENCHIDAS PELA COMERCIAL OSWALDO CRUZ</t>
+        </is>
+      </c>
+      <c r="C58" s="93" t="n"/>
+      <c r="D58" s="93" t="n"/>
+      <c r="E58" s="93" t="n"/>
+      <c r="F58" s="93" t="n"/>
+      <c r="G58" s="93" t="n"/>
+      <c r="H58" s="93" t="n"/>
+      <c r="I58" s="93" t="n"/>
+      <c r="J58" s="94" t="n"/>
+    </row>
+    <row r="59" ht="18" customHeight="1">
+      <c r="B59" s="5" t="inlineStr">
+        <is>
+          <t>COMPRADOR:</t>
+        </is>
+      </c>
+      <c r="C59" s="34" t="n"/>
+      <c r="D59" s="99" t="n"/>
+      <c r="E59" s="99" t="n"/>
+      <c r="F59" s="99" t="n"/>
+      <c r="G59" s="99" t="n"/>
+      <c r="H59" s="99" t="n"/>
+      <c r="I59" s="99" t="n"/>
+      <c r="J59" s="101" t="n"/>
+    </row>
+    <row r="60" ht="18" customFormat="1" customHeight="1" s="9">
+      <c r="B60" s="3" t="inlineStr">
+        <is>
+          <t>MAPA:</t>
+        </is>
+      </c>
+      <c r="C60" s="41" t="inlineStr">
+        <is>
+          <t>A GRANDE (  )</t>
+        </is>
+      </c>
+      <c r="D60" s="115" t="n"/>
+      <c r="E60" s="41" t="inlineStr">
+        <is>
+          <t>A PEQUENO (  )</t>
+        </is>
+      </c>
+      <c r="F60" s="115" t="n"/>
+      <c r="G60" s="41" t="inlineStr">
+        <is>
+          <t>C GRANDE (  )</t>
+        </is>
+      </c>
+      <c r="H60" s="115" t="n"/>
+      <c r="I60" s="41" t="inlineStr">
+        <is>
+          <t>C PEQUENO (  )</t>
+        </is>
+      </c>
+      <c r="J60" s="14" t="n"/>
+    </row>
+    <row r="61" ht="18" customFormat="1" customHeight="1" s="9">
+      <c r="B61" s="5" t="inlineStr">
+        <is>
+          <t>ESTOQUES MÍNIMO E MÁXIMO:</t>
+        </is>
+      </c>
+      <c r="C61" s="6" t="inlineStr">
+        <is>
+          <t>MÍN:</t>
+        </is>
+      </c>
+      <c r="D61" s="6" t="inlineStr">
+        <is>
+          <t>MÁX:</t>
+        </is>
+      </c>
+      <c r="E61" s="6" t="inlineStr">
+        <is>
+          <t>MÍN:</t>
+        </is>
+      </c>
+      <c r="F61" s="6" t="inlineStr">
+        <is>
+          <t>MÁX:</t>
+        </is>
+      </c>
+      <c r="G61" s="6" t="inlineStr">
+        <is>
+          <t>MÍN:</t>
+        </is>
+      </c>
+      <c r="H61" s="6" t="inlineStr">
+        <is>
+          <t>MÁX:</t>
+        </is>
+      </c>
+      <c r="I61" s="6" t="inlineStr">
+        <is>
+          <t>MÍN:</t>
+        </is>
+      </c>
+      <c r="J61" s="15" t="inlineStr">
+        <is>
+          <t>MÁX:</t>
+        </is>
+      </c>
+    </row>
+    <row r="62" ht="18" customHeight="1">
+      <c r="B62" s="3" t="inlineStr">
+        <is>
+          <t>DISTRIBUIDO POR:</t>
+        </is>
+      </c>
+      <c r="C62" s="4" t="inlineStr">
+        <is>
+          <t>MATRIZ (  )</t>
+        </is>
+      </c>
+      <c r="D62" s="4" t="inlineStr">
+        <is>
+          <t>LOJA 05 (  )</t>
+        </is>
+      </c>
+      <c r="E62" s="4" t="inlineStr">
+        <is>
+          <t>LOJA 07 (  )</t>
+        </is>
+      </c>
+      <c r="F62" s="4" t="inlineStr">
+        <is>
+          <t>LOJA 20 (  )</t>
+        </is>
+      </c>
+      <c r="G62" s="4" t="inlineStr">
+        <is>
+          <t>LOJA 11(  )</t>
+        </is>
+      </c>
+      <c r="H62" s="4" t="n"/>
+      <c r="I62" s="4" t="n"/>
+      <c r="J62" s="14" t="n"/>
+    </row>
+    <row r="63" ht="18" customHeight="1">
+      <c r="B63" s="5" t="inlineStr">
+        <is>
+          <t>FORMA DE ABASTECIMENTO:</t>
+        </is>
+      </c>
+      <c r="C63" s="30" t="inlineStr">
+        <is>
+          <t>CENTRAL - CENTRAL (  )</t>
+        </is>
+      </c>
+      <c r="D63" s="115" t="n"/>
+      <c r="E63" s="30" t="inlineStr">
+        <is>
+          <t>CENTRAL - LOJA (  )</t>
+        </is>
+      </c>
+      <c r="F63" s="115" t="n"/>
+      <c r="G63" s="30" t="inlineStr">
+        <is>
+          <t>LOJA - LOJA (  )</t>
+        </is>
+      </c>
+      <c r="H63" s="115" t="n"/>
+      <c r="I63" s="30" t="inlineStr">
+        <is>
+          <t>CROSSDOCKING (  )</t>
+        </is>
+      </c>
+      <c r="J63" s="115" t="n"/>
+    </row>
+    <row r="64" ht="18" customHeight="1">
+      <c r="B64" s="3" t="inlineStr">
+        <is>
+          <t>JÁ EXISTE FAMÍLIA CADASTRADA?</t>
+        </is>
+      </c>
+      <c r="C64" s="32" t="n"/>
+      <c r="D64" s="99" t="n"/>
+      <c r="E64" s="99" t="n"/>
+      <c r="F64" s="99" t="n"/>
+      <c r="G64" s="99" t="n"/>
+      <c r="H64" s="99" t="n"/>
+      <c r="I64" s="99" t="n"/>
+      <c r="J64" s="101" t="n"/>
+    </row>
+    <row r="65" ht="18" customHeight="1">
+      <c r="B65" s="5" t="inlineStr">
+        <is>
+          <t>INFORME O CÓDIGO DA FAMÍLIA:</t>
+        </is>
+      </c>
+      <c r="C65" s="34" t="n"/>
+      <c r="D65" s="99" t="n"/>
+      <c r="E65" s="99" t="n"/>
+      <c r="F65" s="99" t="n"/>
+      <c r="G65" s="99" t="n"/>
+      <c r="H65" s="99" t="n"/>
+      <c r="I65" s="99" t="n"/>
+      <c r="J65" s="101" t="n"/>
+    </row>
+    <row r="66" ht="18" customHeight="1" thickBot="1">
+      <c r="B66" s="7" t="inlineStr">
+        <is>
+          <t>SEGMENTAÇÃO:</t>
+        </is>
+      </c>
+      <c r="C66" s="25" t="n"/>
+      <c r="D66" s="106" t="n"/>
+      <c r="E66" s="106" t="n"/>
+      <c r="F66" s="106" t="n"/>
+      <c r="G66" s="106" t="n"/>
+      <c r="H66" s="106" t="n"/>
+      <c r="I66" s="106" t="n"/>
+      <c r="J66" s="107" t="n"/>
+    </row>
+    <row r="67" ht="18" customHeight="1" thickBot="1">
+      <c r="B67" s="9" t="n"/>
+      <c r="E67" s="9" t="n"/>
+      <c r="F67" s="10" t="n"/>
+      <c r="G67" s="10" t="n"/>
+      <c r="H67" s="10" t="n"/>
+      <c r="I67" s="10" t="n"/>
+    </row>
+    <row r="68" ht="18" customHeight="1" thickBot="1">
+      <c r="B68" s="116" t="inlineStr">
+        <is>
+          <t>ATENÇÃO: TODO PRODUTO NOVO PRECISA DE UMA DIVISÃO INICIAL FEITA PELO COMPRADOR</t>
+        </is>
+      </c>
+      <c r="C68" s="117" t="n"/>
+      <c r="D68" s="117" t="n"/>
+      <c r="E68" s="117" t="n"/>
+      <c r="F68" s="117" t="n"/>
+      <c r="G68" s="117" t="n"/>
+      <c r="H68" s="117" t="n"/>
+      <c r="I68" s="117" t="n"/>
+      <c r="J68" s="118" t="n"/>
+    </row>
+    <row r="69" ht="18" customHeight="1"/>
+    <row r="70" ht="18" customHeight="1"/>
+    <row r="71" ht="18" customHeight="1">
+      <c r="B71" s="16" t="inlineStr">
+        <is>
+          <t>DATA</t>
+        </is>
+      </c>
+      <c r="C71" s="9" t="n"/>
+      <c r="D71" s="16" t="inlineStr">
+        <is>
+          <t>COMPRADOR</t>
+        </is>
+      </c>
+      <c r="E71" s="16" t="n"/>
+      <c r="F71" s="9" t="n"/>
+      <c r="G71" s="9" t="n"/>
+      <c r="H71" s="16" t="inlineStr">
+        <is>
+          <t>GERENTE COMPRAS</t>
+        </is>
+      </c>
+      <c r="I71" s="16" t="n"/>
+      <c r="J71" s="9" t="n"/>
+    </row>
+  </sheetData>
+  <mergeCells count="87">
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C33:J33"/>
+    <mergeCell ref="F10:J10"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="F6:J6"/>
+    <mergeCell ref="C20:J20"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="E63:F63"/>
+    <mergeCell ref="F18:J18"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="F8:J8"/>
+    <mergeCell ref="F17:J17"/>
+    <mergeCell ref="C59:J59"/>
+    <mergeCell ref="C52:J52"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F9:J9"/>
+    <mergeCell ref="B25:J25"/>
+    <mergeCell ref="C48:J48"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="C32:J32"/>
+    <mergeCell ref="F7:J7"/>
+    <mergeCell ref="C26:J26"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="F51:J51"/>
+    <mergeCell ref="C16:J16"/>
+    <mergeCell ref="C50:J50"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="B15:J15"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C28:J28"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="G60:H60"/>
+    <mergeCell ref="B58:J58"/>
+    <mergeCell ref="C30:J30"/>
+    <mergeCell ref="B42:J42"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="C64:J64"/>
+    <mergeCell ref="F55:J55"/>
+    <mergeCell ref="F12:J12"/>
+    <mergeCell ref="B35:J36"/>
+    <mergeCell ref="C54:J54"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C43:J43"/>
+    <mergeCell ref="F23:J23"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C27:J27"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="B46:J46"/>
+    <mergeCell ref="G63:H63"/>
+    <mergeCell ref="I63:J63"/>
+    <mergeCell ref="C66:J66"/>
+    <mergeCell ref="C19:J19"/>
+    <mergeCell ref="C53:J53"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C29:J29"/>
+    <mergeCell ref="C65:J65"/>
+    <mergeCell ref="C47:J47"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C44:J44"/>
+    <mergeCell ref="C22:J22"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="C31:J31"/>
+    <mergeCell ref="B68:J68"/>
+    <mergeCell ref="C21:J21"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="F13:J13"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="F56:J56"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="C49:J49"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
+  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B1:N71"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="1.5703125" customWidth="1" style="1" min="1" max="1"/>
+    <col width="33.28515625" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
+    <col width="15.7109375" customWidth="1" style="1" min="3" max="3"/>
+    <col width="14.7109375" customWidth="1" style="1" min="4" max="4"/>
+    <col width="23.7109375" customWidth="1" style="1" min="5" max="5"/>
+    <col width="14.7109375" customWidth="1" style="1" min="6" max="9"/>
+    <col width="11.5703125" customWidth="1" style="1" min="10" max="10"/>
+    <col width="9.140625" customWidth="1" style="1" min="11" max="16384"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="44.25" customHeight="1" thickBot="1">
+      <c r="B1" s="90" t="inlineStr">
+        <is>
+          <t>CADASTRO SUPERMERCADOS JOANIN LTDA</t>
+        </is>
+      </c>
+      <c r="C1" s="91" t="n"/>
+      <c r="D1" s="91" t="n"/>
+      <c r="E1" s="91" t="n"/>
+      <c r="F1" s="91" t="n"/>
+      <c r="G1" s="91" t="n"/>
+      <c r="H1" s="91" t="n"/>
+      <c r="I1" s="91" t="n"/>
+      <c r="J1" s="92" t="n"/>
+    </row>
+    <row r="2" ht="18" customHeight="1" thickBot="1"/>
+    <row r="3" ht="18" customHeight="1">
+      <c r="B3" s="38" t="inlineStr">
+        <is>
+          <t>INFORMAÇÕES FORNECEDOR</t>
+        </is>
+      </c>
+      <c r="C3" s="93" t="n"/>
+      <c r="D3" s="93" t="n"/>
+      <c r="E3" s="93" t="n"/>
+      <c r="F3" s="93" t="n"/>
+      <c r="G3" s="93" t="n"/>
+      <c r="H3" s="93" t="n"/>
+      <c r="I3" s="93" t="n"/>
+      <c r="J3" s="94" t="n"/>
+    </row>
+    <row r="4" ht="18" customHeight="1">
+      <c r="B4" s="95" t="inlineStr">
+        <is>
+          <t>É FORNECEDOR NOVO (    ) SIM     (   ) NÃO                           -                            FOI FEITO CONTRATO (   ) SIM      (    ) NÃO</t>
+        </is>
+      </c>
+      <c r="C4" s="96" t="n"/>
+      <c r="D4" s="96" t="n"/>
+      <c r="E4" s="96" t="n"/>
+      <c r="F4" s="96" t="n"/>
+      <c r="G4" s="96" t="n"/>
+      <c r="H4" s="96" t="n"/>
+      <c r="I4" s="96" t="n"/>
+      <c r="J4" s="97" t="n"/>
+    </row>
+    <row r="5" ht="18" customHeight="1">
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>RAZÃO SOCIAL:</t>
+        </is>
+      </c>
+      <c r="C5" s="98" t="inlineStr">
+        <is>
+          <t>NETFEIRA PONTOCOM LTDA</t>
+        </is>
+      </c>
+      <c r="D5" s="99" t="n"/>
+      <c r="E5" s="99" t="n"/>
+      <c r="F5" s="99" t="n"/>
+      <c r="G5" s="99" t="n"/>
+      <c r="H5" s="99" t="n"/>
+      <c r="I5" s="99" t="n"/>
+      <c r="J5" s="100" t="n"/>
+    </row>
+    <row r="6" ht="18" customHeight="1">
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+      <c r="C6" s="51" t="inlineStr">
+        <is>
+          <t>03.974.724/0001-24</t>
+        </is>
+      </c>
+      <c r="D6" s="101" t="n"/>
+      <c r="E6" s="4" t="inlineStr">
+        <is>
+          <t>INSC. ESTADUAL:</t>
+        </is>
+      </c>
+      <c r="F6" s="72" t="inlineStr">
+        <is>
+          <t>115.951.284-113</t>
+        </is>
+      </c>
+      <c r="G6" s="99" t="n"/>
+      <c r="H6" s="99" t="n"/>
+      <c r="I6" s="99" t="n"/>
+      <c r="J6" s="101" t="n"/>
+    </row>
+    <row r="7" ht="18" customHeight="1">
+      <c r="B7" s="5" t="inlineStr">
+        <is>
+          <t>ENDEREÇO:</t>
+        </is>
+      </c>
+      <c r="C7" s="71" t="inlineStr">
+        <is>
+          <t>AVENIDA DOUTOR GASTÃO VIDIGAL</t>
+        </is>
+      </c>
+      <c r="D7" s="101" t="n"/>
+      <c r="E7" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nº </t>
+        </is>
+      </c>
+      <c r="F7" s="72" t="inlineStr">
+        <is>
+          <t>1946</t>
+        </is>
+      </c>
+      <c r="G7" s="99" t="n"/>
+      <c r="H7" s="99" t="n"/>
+      <c r="I7" s="99" t="n"/>
+      <c r="J7" s="101" t="n"/>
+    </row>
+    <row r="8" ht="18" customHeight="1">
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BAIRRO: </t>
+        </is>
+      </c>
+      <c r="C8" s="51" t="inlineStr">
+        <is>
+          <t>VILA LEOPOLDINA</t>
+        </is>
+      </c>
+      <c r="D8" s="101" t="n"/>
+      <c r="E8" s="4" t="inlineStr">
+        <is>
+          <t>CEP:</t>
+        </is>
+      </c>
+      <c r="F8" s="72" t="inlineStr">
+        <is>
+          <t>5316900</t>
+        </is>
+      </c>
+      <c r="G8" s="99" t="n"/>
+      <c r="H8" s="99" t="n"/>
+      <c r="I8" s="99" t="n"/>
+      <c r="J8" s="101" t="n"/>
+    </row>
+    <row r="9" ht="18" customHeight="1">
+      <c r="B9" s="5" t="inlineStr">
+        <is>
+          <t>CIDADE:</t>
+        </is>
+      </c>
+      <c r="C9" s="34" t="inlineStr">
+        <is>
+          <t>SÃO PAULO</t>
+        </is>
+      </c>
+      <c r="D9" s="101" t="n"/>
+      <c r="E9" s="6" t="inlineStr">
+        <is>
+          <t>ESTADO:</t>
+        </is>
+      </c>
+      <c r="F9" s="71" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="G9" s="99" t="n"/>
+      <c r="H9" s="99" t="n"/>
+      <c r="I9" s="99" t="n"/>
+      <c r="J9" s="101" t="n"/>
+    </row>
+    <row r="10" ht="18" customHeight="1">
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>COMPLEMENTO:</t>
+        </is>
+      </c>
+      <c r="C10" s="51" t="inlineStr">
+        <is>
+          <t>P.AMA BOX 61/62,AMB BOX 3,4</t>
+        </is>
+      </c>
+      <c r="D10" s="101" t="n"/>
+      <c r="E10" s="19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PRAZO DE PGTO </t>
+        </is>
+      </c>
+      <c r="F10" s="102" t="n"/>
+      <c r="G10" s="99" t="n"/>
+      <c r="H10" s="99" t="n"/>
+      <c r="I10" s="99" t="n"/>
+      <c r="J10" s="100" t="n"/>
+    </row>
+    <row r="11" ht="18" customHeight="1">
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>CONTATO :</t>
+        </is>
+      </c>
+      <c r="C11" s="51" t="n"/>
+      <c r="D11" s="101" t="n"/>
+      <c r="E11" s="4" t="inlineStr">
+        <is>
+          <t>TELEFONE :</t>
+        </is>
+      </c>
+      <c r="F11" s="75" t="n"/>
+      <c r="G11" s="76" t="n"/>
+      <c r="H11" s="76" t="n"/>
+      <c r="I11" s="76" t="n"/>
+      <c r="J11" s="77" t="n"/>
+    </row>
+    <row r="12" ht="18" customHeight="1">
+      <c r="B12" s="23" t="inlineStr">
+        <is>
+          <t>E-MAIL PARA ENVIO XML</t>
+        </is>
+      </c>
+      <c r="C12" s="78" t="n"/>
+      <c r="D12" s="101" t="n"/>
+      <c r="E12" s="24" t="inlineStr">
+        <is>
+          <t>E-MAIL PARA FINANCEIRO</t>
+        </is>
+      </c>
+      <c r="F12" s="80" t="n"/>
+      <c r="G12" s="99" t="n"/>
+      <c r="H12" s="99" t="n"/>
+      <c r="I12" s="99" t="n"/>
+      <c r="J12" s="101" t="n"/>
+    </row>
+    <row r="13" ht="18" customHeight="1" thickBot="1">
+      <c r="B13" s="67" t="inlineStr">
+        <is>
+          <t>(    )COM INDENIZAÇÃO - FORNECEDOR ACEITA NOTA FISCAL DE DEVOLUÇÃO</t>
+        </is>
+      </c>
+      <c r="C13" s="103" t="n"/>
+      <c r="D13" s="103" t="n"/>
+      <c r="E13" s="103" t="n"/>
+      <c r="F13" s="70" t="inlineStr">
+        <is>
+          <t>(    ) SEM INDENIZAÇÃO  -  FORNECEDOR NÃO ACEITA NOTA FISCAL DEVOLUÇÃO</t>
+        </is>
+      </c>
+      <c r="G13" s="104" t="n"/>
+      <c r="H13" s="104" t="n"/>
+      <c r="I13" s="104" t="n"/>
+      <c r="J13" s="105" t="n"/>
+    </row>
+    <row r="14" ht="18" customHeight="1" thickBot="1">
+      <c r="B14" s="9" t="n"/>
+      <c r="E14" s="9" t="n"/>
+      <c r="F14" s="10" t="n"/>
+      <c r="G14" s="10" t="n"/>
+      <c r="H14" s="10" t="n"/>
+      <c r="I14" s="10" t="n"/>
+    </row>
+    <row r="15" ht="18" customHeight="1">
+      <c r="B15" s="38" t="inlineStr">
+        <is>
+          <t>DADOS DO PRODUTO - UNIDADE</t>
+        </is>
+      </c>
+      <c r="C15" s="93" t="n"/>
+      <c r="D15" s="93" t="n"/>
+      <c r="E15" s="93" t="n"/>
+      <c r="F15" s="93" t="n"/>
+      <c r="G15" s="93" t="n"/>
+      <c r="H15" s="93" t="n"/>
+      <c r="I15" s="93" t="n"/>
+      <c r="J15" s="94" t="n"/>
+    </row>
+    <row r="16" ht="18" customHeight="1">
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t>DESCRIÇÃO:</t>
+        </is>
+      </c>
+      <c r="C16" s="32" t="inlineStr">
+        <is>
+          <t>AÇAI BUFALO COM BANANA CONGELADO 1,300KG</t>
+        </is>
+      </c>
+      <c r="D16" s="99" t="n"/>
+      <c r="E16" s="99" t="n"/>
+      <c r="F16" s="99" t="n"/>
+      <c r="G16" s="99" t="n"/>
+      <c r="H16" s="99" t="n"/>
+      <c r="I16" s="99" t="n"/>
+      <c r="J16" s="101" t="n"/>
+      <c r="N16" s="11" t="n"/>
+    </row>
+    <row r="17" ht="18" customHeight="1">
+      <c r="B17" s="5" t="inlineStr">
+        <is>
+          <t>CÓD DE BARRAS:</t>
+        </is>
+      </c>
+      <c r="C17" s="65" t="inlineStr">
+        <is>
+          <t>7896519298662</t>
+        </is>
+      </c>
+      <c r="D17" s="101" t="n"/>
+      <c r="E17" s="12" t="inlineStr">
+        <is>
+          <t>MARCA:</t>
+        </is>
+      </c>
+      <c r="F17" s="65" t="inlineStr">
+        <is>
+          <t>DE MARCHI</t>
+        </is>
+      </c>
+      <c r="G17" s="99" t="n"/>
+      <c r="H17" s="99" t="n"/>
+      <c r="I17" s="99" t="n"/>
+      <c r="J17" s="101" t="n"/>
+    </row>
+    <row r="18" ht="18" customHeight="1">
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>PESO LIQUIDO KG:</t>
+        </is>
+      </c>
+      <c r="C18" s="51" t="inlineStr">
+        <is>
+          <t>1.3</t>
+        </is>
+      </c>
+      <c r="D18" s="101" t="n"/>
+      <c r="E18" s="4" t="inlineStr">
+        <is>
+          <t>PESO BRUTO KG:</t>
+        </is>
+      </c>
+      <c r="F18" s="32" t="inlineStr">
+        <is>
+          <t>1.3</t>
+        </is>
+      </c>
+      <c r="G18" s="99" t="n"/>
+      <c r="H18" s="99" t="n"/>
+      <c r="I18" s="99" t="n"/>
+      <c r="J18" s="101" t="n"/>
+    </row>
+    <row r="19" ht="18" customHeight="1">
+      <c r="B19" s="5" t="inlineStr">
+        <is>
+          <t>COMPRIMENTO EM CM:</t>
+        </is>
+      </c>
+      <c r="C19" s="34" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D19" s="99" t="n"/>
+      <c r="E19" s="99" t="n"/>
+      <c r="F19" s="99" t="n"/>
+      <c r="G19" s="99" t="n"/>
+      <c r="H19" s="99" t="n"/>
+      <c r="I19" s="99" t="n"/>
+      <c r="J19" s="101" t="n"/>
+    </row>
+    <row r="20" ht="18" customHeight="1">
+      <c r="B20" s="3" t="inlineStr">
+        <is>
+          <t>LARGURA EM CM:</t>
+        </is>
+      </c>
+      <c r="C20" s="57" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D20" s="99" t="n"/>
+      <c r="E20" s="99" t="n"/>
+      <c r="F20" s="99" t="n"/>
+      <c r="G20" s="99" t="n"/>
+      <c r="H20" s="99" t="n"/>
+      <c r="I20" s="99" t="n"/>
+      <c r="J20" s="101" t="n"/>
+    </row>
+    <row r="21" ht="18" customHeight="1">
+      <c r="B21" s="5" t="inlineStr">
+        <is>
+          <t>ALTURA EM CM:</t>
+        </is>
+      </c>
+      <c r="C21" s="59" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D21" s="99" t="n"/>
+      <c r="E21" s="99" t="n"/>
+      <c r="F21" s="99" t="n"/>
+      <c r="G21" s="99" t="n"/>
+      <c r="H21" s="99" t="n"/>
+      <c r="I21" s="99" t="n"/>
+      <c r="J21" s="101" t="n"/>
+    </row>
+    <row r="22" ht="18" customHeight="1">
+      <c r="B22" s="3" t="inlineStr">
+        <is>
+          <t>VALIDADE EM DIAS:</t>
+        </is>
+      </c>
+      <c r="C22" s="32" t="n"/>
+      <c r="D22" s="99" t="n"/>
+      <c r="E22" s="99" t="n"/>
+      <c r="F22" s="99" t="n"/>
+      <c r="G22" s="99" t="n"/>
+      <c r="H22" s="99" t="n"/>
+      <c r="I22" s="99" t="n"/>
+      <c r="J22" s="101" t="n"/>
+    </row>
+    <row r="23" ht="18" customHeight="1" thickBot="1">
+      <c r="B23" s="7" t="inlineStr">
+        <is>
+          <t>COD PRODUTO FORNECEDOR:</t>
+        </is>
+      </c>
+      <c r="C23" s="25" t="inlineStr">
+        <is>
+          <t>9634</t>
+        </is>
+      </c>
+      <c r="D23" s="106" t="n"/>
+      <c r="E23" s="107" t="n"/>
+      <c r="F23" s="61" t="inlineStr">
+        <is>
+          <t>(É OBRIGADOTÓRIO QUE O CÓDIGO DO FORNECEDOR SEJA O MESMO DO XML)</t>
+        </is>
+      </c>
+      <c r="G23" s="106" t="n"/>
+      <c r="H23" s="106" t="n"/>
+      <c r="I23" s="106" t="n"/>
+      <c r="J23" s="107" t="n"/>
+    </row>
+    <row r="24" ht="18" customHeight="1" thickBot="1"/>
+    <row r="25" ht="18" customHeight="1">
+      <c r="B25" s="38" t="inlineStr">
+        <is>
+          <t>DADOS DO PRODUTO - CAIXA</t>
+        </is>
+      </c>
+      <c r="C25" s="93" t="n"/>
+      <c r="D25" s="93" t="n"/>
+      <c r="E25" s="93" t="n"/>
+      <c r="F25" s="93" t="n"/>
+      <c r="G25" s="93" t="n"/>
+      <c r="H25" s="93" t="n"/>
+      <c r="I25" s="93" t="n"/>
+      <c r="J25" s="94" t="n"/>
+    </row>
+    <row r="26" ht="18" customHeight="1">
+      <c r="B26" s="3" t="inlineStr">
+        <is>
+          <t>TIPO DE EMBALAGEM:</t>
+        </is>
+      </c>
+      <c r="C26" s="32" t="inlineStr">
+        <is>
+          <t>UN</t>
+        </is>
+      </c>
+      <c r="D26" s="99" t="n"/>
+      <c r="E26" s="99" t="n"/>
+      <c r="F26" s="99" t="n"/>
+      <c r="G26" s="99" t="n"/>
+      <c r="H26" s="99" t="n"/>
+      <c r="I26" s="99" t="n"/>
+      <c r="J26" s="101" t="n"/>
+    </row>
+    <row r="27" ht="18" customHeight="1">
+      <c r="B27" s="5" t="inlineStr">
+        <is>
+          <t>QUANTIDADE NA CAIXA:</t>
+        </is>
+      </c>
+      <c r="C27" s="34" t="inlineStr">
+        <is>
+          <t>6.0</t>
+        </is>
+      </c>
+      <c r="D27" s="99" t="n"/>
+      <c r="E27" s="99" t="n"/>
+      <c r="F27" s="99" t="n"/>
+      <c r="G27" s="99" t="n"/>
+      <c r="H27" s="99" t="n"/>
+      <c r="I27" s="99" t="n"/>
+      <c r="J27" s="101" t="n"/>
+    </row>
+    <row r="28" ht="18" customHeight="1">
+      <c r="B28" s="3" t="inlineStr">
+        <is>
+          <t>CÓD DUN:</t>
+        </is>
+      </c>
+      <c r="C28" s="63" t="inlineStr">
+        <is>
+          <t>67896519298664</t>
+        </is>
+      </c>
+      <c r="D28" s="99" t="n"/>
+      <c r="E28" s="99" t="n"/>
+      <c r="F28" s="99" t="n"/>
+      <c r="G28" s="99" t="n"/>
+      <c r="H28" s="99" t="n"/>
+      <c r="I28" s="99" t="n"/>
+      <c r="J28" s="101" t="n"/>
+    </row>
+    <row r="29" ht="18" customHeight="1">
+      <c r="B29" s="5" t="inlineStr">
+        <is>
+          <t>PESO BRUTO KG:</t>
+        </is>
+      </c>
+      <c r="C29" s="34" t="inlineStr">
+        <is>
+          <t>7.8</t>
+        </is>
+      </c>
+      <c r="D29" s="99" t="n"/>
+      <c r="E29" s="99" t="n"/>
+      <c r="F29" s="99" t="n"/>
+      <c r="G29" s="99" t="n"/>
+      <c r="H29" s="99" t="n"/>
+      <c r="I29" s="99" t="n"/>
+      <c r="J29" s="101" t="n"/>
+    </row>
+    <row r="30" ht="18" customHeight="1">
+      <c r="B30" s="3" t="inlineStr">
+        <is>
+          <t>PESO LIQUIDO KG:</t>
+        </is>
+      </c>
+      <c r="C30" s="32" t="inlineStr">
+        <is>
+          <t>7.8</t>
+        </is>
+      </c>
+      <c r="D30" s="99" t="n"/>
+      <c r="E30" s="99" t="n"/>
+      <c r="F30" s="99" t="n"/>
+      <c r="G30" s="99" t="n"/>
+      <c r="H30" s="99" t="n"/>
+      <c r="I30" s="99" t="n"/>
+      <c r="J30" s="101" t="n"/>
+    </row>
+    <row r="31" ht="18" customHeight="1">
+      <c r="B31" s="5" t="inlineStr">
+        <is>
+          <t>COMPRIMENTO EM CM:</t>
+        </is>
+      </c>
+      <c r="C31" s="34" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D31" s="99" t="n"/>
+      <c r="E31" s="99" t="n"/>
+      <c r="F31" s="99" t="n"/>
+      <c r="G31" s="99" t="n"/>
+      <c r="H31" s="99" t="n"/>
+      <c r="I31" s="99" t="n"/>
+      <c r="J31" s="101" t="n"/>
+    </row>
+    <row r="32" ht="18" customHeight="1">
+      <c r="B32" s="3" t="inlineStr">
+        <is>
+          <t>LARGURA EM CM:</t>
+        </is>
+      </c>
+      <c r="C32" s="32" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D32" s="99" t="n"/>
+      <c r="E32" s="99" t="n"/>
+      <c r="F32" s="99" t="n"/>
+      <c r="G32" s="99" t="n"/>
+      <c r="H32" s="99" t="n"/>
+      <c r="I32" s="99" t="n"/>
+      <c r="J32" s="101" t="n"/>
+    </row>
+    <row r="33" ht="18" customHeight="1" thickBot="1">
+      <c r="B33" s="7" t="inlineStr">
+        <is>
+          <t>ALTURA EM CM:</t>
+        </is>
+      </c>
+      <c r="C33" s="25" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D33" s="106" t="n"/>
+      <c r="E33" s="106" t="n"/>
+      <c r="F33" s="106" t="n"/>
+      <c r="G33" s="106" t="n"/>
+      <c r="H33" s="106" t="n"/>
+      <c r="I33" s="106" t="n"/>
+      <c r="J33" s="107" t="n"/>
+    </row>
+    <row r="34" ht="18" customHeight="1" thickBot="1"/>
+    <row r="35" ht="18" customHeight="1">
+      <c r="B35" s="38" t="inlineStr">
+        <is>
+          <t>CUSTO DO PRODUTO - UNITÁRIO</t>
+        </is>
+      </c>
+      <c r="C35" s="108" t="n"/>
+      <c r="D35" s="108" t="n"/>
+      <c r="E35" s="108" t="n"/>
+      <c r="F35" s="108" t="n"/>
+      <c r="G35" s="108" t="n"/>
+      <c r="H35" s="108" t="n"/>
+      <c r="I35" s="108" t="n"/>
+      <c r="J35" s="109" t="n"/>
+    </row>
+    <row r="36" ht="18" customHeight="1">
+      <c r="B36" s="110" t="n"/>
+      <c r="C36" s="111" t="n"/>
+      <c r="D36" s="111" t="n"/>
+      <c r="E36" s="111" t="n"/>
+      <c r="F36" s="111" t="n"/>
+      <c r="G36" s="111" t="n"/>
+      <c r="H36" s="111" t="n"/>
+      <c r="I36" s="111" t="n"/>
+      <c r="J36" s="112" t="n"/>
+    </row>
+    <row r="37" ht="18" customHeight="1">
+      <c r="B37" s="17" t="inlineStr">
+        <is>
+          <t>CUSTO SEM ST:</t>
+        </is>
+      </c>
+      <c r="C37" s="51" t="n"/>
+      <c r="D37" s="101" t="n"/>
+      <c r="E37" s="52" t="inlineStr">
+        <is>
+          <t>CUSTO COM ST:</t>
+        </is>
+      </c>
+      <c r="F37" s="113" t="n"/>
+      <c r="G37" s="51" t="n"/>
+      <c r="H37" s="101" t="n"/>
+      <c r="I37" s="52" t="n"/>
+      <c r="J37" s="113" t="n"/>
+    </row>
+    <row r="38" ht="18" customHeight="1">
+      <c r="B38" s="17" t="inlineStr">
+        <is>
+          <t>VALOR DA ST:</t>
+        </is>
+      </c>
+      <c r="C38" s="51" t="n"/>
+      <c r="D38" s="101" t="n"/>
+      <c r="E38" s="52" t="inlineStr">
+        <is>
+          <t>CUSTO UNITÁRIO FINAL:</t>
+        </is>
+      </c>
+      <c r="F38" s="113" t="n"/>
+      <c r="G38" s="51" t="n"/>
+      <c r="H38" s="101" t="n"/>
+      <c r="I38" s="52" t="n"/>
+      <c r="J38" s="113" t="n"/>
+    </row>
+    <row r="39" ht="18" customHeight="1">
+      <c r="B39" s="17" t="inlineStr">
+        <is>
+          <t>VERBA:</t>
+        </is>
+      </c>
+      <c r="C39" s="51" t="n"/>
+      <c r="D39" s="101" t="n"/>
+      <c r="E39" s="52" t="inlineStr">
+        <is>
+          <t>MARGEM:</t>
+        </is>
+      </c>
+      <c r="F39" s="113" t="n"/>
+      <c r="G39" s="51" t="n"/>
+      <c r="H39" s="101" t="n"/>
+      <c r="I39" s="52" t="n"/>
+      <c r="J39" s="113" t="n"/>
+    </row>
+    <row r="40" ht="18" customHeight="1" thickBot="1">
+      <c r="B40" s="18" t="n"/>
+      <c r="C40" s="53" t="n"/>
+      <c r="D40" s="107" t="n"/>
+      <c r="E40" s="54" t="inlineStr">
+        <is>
+          <t>VALOR DE VENDA:</t>
+        </is>
+      </c>
+      <c r="F40" s="114" t="n"/>
+      <c r="G40" s="53" t="n"/>
+      <c r="H40" s="107" t="n"/>
+      <c r="I40" s="54" t="n"/>
+      <c r="J40" s="114" t="n"/>
+    </row>
+    <row r="41" ht="18" customHeight="1" thickBot="1"/>
+    <row r="42" ht="18" customHeight="1">
+      <c r="B42" s="38" t="inlineStr">
+        <is>
+          <t>DADOS PALLETIZAÇÃO</t>
+        </is>
+      </c>
+      <c r="C42" s="93" t="n"/>
+      <c r="D42" s="93" t="n"/>
+      <c r="E42" s="93" t="n"/>
+      <c r="F42" s="93" t="n"/>
+      <c r="G42" s="93" t="n"/>
+      <c r="H42" s="93" t="n"/>
+      <c r="I42" s="93" t="n"/>
+      <c r="J42" s="94" t="n"/>
+    </row>
+    <row r="43" ht="18" customHeight="1">
+      <c r="B43" s="3" t="inlineStr">
+        <is>
+          <t>LASTRO/CAMADA:</t>
+        </is>
+      </c>
+      <c r="C43" s="32" t="n"/>
+      <c r="D43" s="99" t="n"/>
+      <c r="E43" s="99" t="n"/>
+      <c r="F43" s="99" t="n"/>
+      <c r="G43" s="99" t="n"/>
+      <c r="H43" s="99" t="n"/>
+      <c r="I43" s="99" t="n"/>
+      <c r="J43" s="101" t="n"/>
+    </row>
+    <row r="44" ht="18" customHeight="1" thickBot="1">
+      <c r="B44" s="7" t="inlineStr">
+        <is>
+          <t>ALTURA:</t>
+        </is>
+      </c>
+      <c r="C44" s="25" t="n"/>
+      <c r="D44" s="106" t="n"/>
+      <c r="E44" s="106" t="n"/>
+      <c r="F44" s="106" t="n"/>
+      <c r="G44" s="106" t="n"/>
+      <c r="H44" s="106" t="n"/>
+      <c r="I44" s="106" t="n"/>
+      <c r="J44" s="107" t="n"/>
+    </row>
+    <row r="45" ht="18" customHeight="1" thickBot="1"/>
+    <row r="46" ht="18" customHeight="1">
+      <c r="B46" s="38" t="inlineStr">
+        <is>
+          <t>INFORMAÇÕES FISCAIS</t>
+        </is>
+      </c>
+      <c r="C46" s="93" t="n"/>
+      <c r="D46" s="93" t="n"/>
+      <c r="E46" s="93" t="n"/>
+      <c r="F46" s="93" t="n"/>
+      <c r="G46" s="93" t="n"/>
+      <c r="H46" s="93" t="n"/>
+      <c r="I46" s="93" t="n"/>
+      <c r="J46" s="94" t="n"/>
+    </row>
+    <row r="47" ht="18" customHeight="1">
+      <c r="B47" s="3" t="inlineStr">
+        <is>
+          <t>NCM:</t>
+        </is>
+      </c>
+      <c r="C47" s="32" t="inlineStr">
+        <is>
+          <t>2106.90.90</t>
+        </is>
+      </c>
+      <c r="D47" s="99" t="n"/>
+      <c r="E47" s="99" t="n"/>
+      <c r="F47" s="99" t="n"/>
+      <c r="G47" s="99" t="n"/>
+      <c r="H47" s="99" t="n"/>
+      <c r="I47" s="99" t="n"/>
+      <c r="J47" s="101" t="n"/>
+    </row>
+    <row r="48" ht="18" customHeight="1">
+      <c r="B48" s="5" t="inlineStr">
+        <is>
+          <t>CEST:</t>
+        </is>
+      </c>
+      <c r="C48" s="34" t="inlineStr">
+        <is>
+          <t>020</t>
         </is>
       </c>
       <c r="D48" s="99" t="n"/>

</xml_diff>